<commit_message>
Update Excel Planung Gantt
</commit_message>
<xml_diff>
--- a/Planung/Tasks&Meilensteine_SA_Stix.xlsx
+++ b/Planung/Tasks&Meilensteine_SA_Stix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kftg-my.sharepoint.com/personal/simeon_stix_stud_kftg_ch/Documents/SA-Dossier 3i V1.4/Planung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simeo\Documents\GitHub\CKi\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{D5EB2CCE-97E9-4532-B27E-A4E376E98DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCE563DE-AA22-4B39-9614-8280124C2614}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EE17D6-21E8-49B3-98A4-BB920CE0F898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="6015" windowWidth="23415" windowHeight="15345" activeTab="1" xr2:uid="{D7FD5909-70C7-4716-9950-CB604D43848C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{D7FD5909-70C7-4716-9950-CB604D43848C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Planung" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="82">
   <si>
     <t>Reserche CNN</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Klassendiagramm</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -496,22 +502,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -880,13 +886,13 @@
       <c r="L1" s="47"/>
       <c r="M1" s="47"/>
       <c r="N1" s="47"/>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
       <c r="T1" s="47">
         <v>45205</v>
       </c>
@@ -901,20 +907,20 @@
       <c r="AA1" s="47"/>
       <c r="AB1" s="47"/>
       <c r="AC1" s="47"/>
-      <c r="AD1" s="48">
+      <c r="AD1" s="49">
         <v>45212</v>
       </c>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48">
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49">
         <v>45213</v>
       </c>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
+      <c r="AM1" s="49"/>
       <c r="AN1" s="47">
         <v>45219</v>
       </c>
@@ -1041,34 +1047,34 @@
       <c r="DW1" s="47"/>
       <c r="DX1" s="47"/>
       <c r="DY1" s="47"/>
-      <c r="DZ1" s="48">
+      <c r="DZ1" s="49">
         <v>45282</v>
       </c>
-      <c r="EA1" s="48"/>
-      <c r="EB1" s="48"/>
-      <c r="EC1" s="48"/>
-      <c r="ED1" s="48"/>
-      <c r="EE1" s="48">
+      <c r="EA1" s="49"/>
+      <c r="EB1" s="49"/>
+      <c r="EC1" s="49"/>
+      <c r="ED1" s="49"/>
+      <c r="EE1" s="49">
         <v>45283</v>
       </c>
-      <c r="EF1" s="48"/>
-      <c r="EG1" s="48"/>
-      <c r="EH1" s="48"/>
-      <c r="EI1" s="48"/>
-      <c r="EJ1" s="48">
+      <c r="EF1" s="49"/>
+      <c r="EG1" s="49"/>
+      <c r="EH1" s="49"/>
+      <c r="EI1" s="49"/>
+      <c r="EJ1" s="49">
         <v>45289</v>
       </c>
-      <c r="EK1" s="48"/>
-      <c r="EL1" s="48"/>
-      <c r="EM1" s="48"/>
-      <c r="EN1" s="48"/>
-      <c r="EO1" s="48">
+      <c r="EK1" s="49"/>
+      <c r="EL1" s="49"/>
+      <c r="EM1" s="49"/>
+      <c r="EN1" s="49"/>
+      <c r="EO1" s="49">
         <v>45290</v>
       </c>
-      <c r="EP1" s="48"/>
-      <c r="EQ1" s="48"/>
-      <c r="ER1" s="48"/>
-      <c r="ES1" s="48"/>
+      <c r="EP1" s="49"/>
+      <c r="EQ1" s="49"/>
+      <c r="ER1" s="49"/>
+      <c r="ES1" s="49"/>
       <c r="ET1" s="47">
         <v>45296</v>
       </c>
@@ -2229,11 +2235,64 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="75">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="MV1:MZ1"/>
+    <mergeCell ref="NA1:NE1"/>
+    <mergeCell ref="NF1:NJ1"/>
+    <mergeCell ref="NK1:NO1"/>
+    <mergeCell ref="LR1:LV1"/>
+    <mergeCell ref="LW1:MA1"/>
+    <mergeCell ref="MB1:MF1"/>
+    <mergeCell ref="MG1:MK1"/>
+    <mergeCell ref="ML1:MP1"/>
+    <mergeCell ref="MQ1:MU1"/>
+    <mergeCell ref="LM1:LQ1"/>
+    <mergeCell ref="JJ1:JN1"/>
+    <mergeCell ref="JO1:JS1"/>
+    <mergeCell ref="JT1:JX1"/>
+    <mergeCell ref="JY1:KC1"/>
+    <mergeCell ref="KD1:KH1"/>
+    <mergeCell ref="KI1:KM1"/>
+    <mergeCell ref="KN1:KR1"/>
+    <mergeCell ref="KS1:KW1"/>
+    <mergeCell ref="KX1:LB1"/>
+    <mergeCell ref="LC1:LG1"/>
+    <mergeCell ref="LH1:LL1"/>
+    <mergeCell ref="JE1:JI1"/>
+    <mergeCell ref="HB1:HF1"/>
+    <mergeCell ref="HG1:HK1"/>
+    <mergeCell ref="HL1:HP1"/>
+    <mergeCell ref="HQ1:HU1"/>
+    <mergeCell ref="HV1:HZ1"/>
+    <mergeCell ref="IA1:IE1"/>
+    <mergeCell ref="IF1:IJ1"/>
+    <mergeCell ref="IK1:IO1"/>
+    <mergeCell ref="IP1:IT1"/>
+    <mergeCell ref="IU1:IY1"/>
+    <mergeCell ref="IZ1:JD1"/>
+    <mergeCell ref="GW1:HA1"/>
+    <mergeCell ref="ET1:EX1"/>
+    <mergeCell ref="EY1:FC1"/>
+    <mergeCell ref="FD1:FH1"/>
+    <mergeCell ref="FI1:FM1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FS1:FW1"/>
+    <mergeCell ref="FX1:GB1"/>
+    <mergeCell ref="GC1:GG1"/>
+    <mergeCell ref="GH1:GL1"/>
+    <mergeCell ref="GM1:GQ1"/>
+    <mergeCell ref="GR1:GV1"/>
+    <mergeCell ref="EO1:ES1"/>
+    <mergeCell ref="CL1:CP1"/>
+    <mergeCell ref="CQ1:CU1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DA1:DE1"/>
+    <mergeCell ref="DF1:DJ1"/>
+    <mergeCell ref="DK1:DO1"/>
+    <mergeCell ref="DP1:DT1"/>
+    <mergeCell ref="DU1:DY1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="EE1:EI1"/>
+    <mergeCell ref="EJ1:EN1"/>
     <mergeCell ref="CG1:CK1"/>
     <mergeCell ref="AD1:AH1"/>
     <mergeCell ref="AI1:AM1"/>
@@ -2246,64 +2305,11 @@
     <mergeCell ref="BR1:BV1"/>
     <mergeCell ref="BW1:CA1"/>
     <mergeCell ref="CB1:CF1"/>
-    <mergeCell ref="EO1:ES1"/>
-    <mergeCell ref="CL1:CP1"/>
-    <mergeCell ref="CQ1:CU1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DA1:DE1"/>
-    <mergeCell ref="DF1:DJ1"/>
-    <mergeCell ref="DK1:DO1"/>
-    <mergeCell ref="DP1:DT1"/>
-    <mergeCell ref="DU1:DY1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="EE1:EI1"/>
-    <mergeCell ref="EJ1:EN1"/>
-    <mergeCell ref="GW1:HA1"/>
-    <mergeCell ref="ET1:EX1"/>
-    <mergeCell ref="EY1:FC1"/>
-    <mergeCell ref="FD1:FH1"/>
-    <mergeCell ref="FI1:FM1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FS1:FW1"/>
-    <mergeCell ref="FX1:GB1"/>
-    <mergeCell ref="GC1:GG1"/>
-    <mergeCell ref="GH1:GL1"/>
-    <mergeCell ref="GM1:GQ1"/>
-    <mergeCell ref="GR1:GV1"/>
-    <mergeCell ref="JE1:JI1"/>
-    <mergeCell ref="HB1:HF1"/>
-    <mergeCell ref="HG1:HK1"/>
-    <mergeCell ref="HL1:HP1"/>
-    <mergeCell ref="HQ1:HU1"/>
-    <mergeCell ref="HV1:HZ1"/>
-    <mergeCell ref="IA1:IE1"/>
-    <mergeCell ref="IF1:IJ1"/>
-    <mergeCell ref="IK1:IO1"/>
-    <mergeCell ref="IP1:IT1"/>
-    <mergeCell ref="IU1:IY1"/>
-    <mergeCell ref="IZ1:JD1"/>
-    <mergeCell ref="LM1:LQ1"/>
-    <mergeCell ref="JJ1:JN1"/>
-    <mergeCell ref="JO1:JS1"/>
-    <mergeCell ref="JT1:JX1"/>
-    <mergeCell ref="JY1:KC1"/>
-    <mergeCell ref="KD1:KH1"/>
-    <mergeCell ref="KI1:KM1"/>
-    <mergeCell ref="KN1:KR1"/>
-    <mergeCell ref="KS1:KW1"/>
-    <mergeCell ref="KX1:LB1"/>
-    <mergeCell ref="LC1:LG1"/>
-    <mergeCell ref="LH1:LL1"/>
-    <mergeCell ref="MV1:MZ1"/>
-    <mergeCell ref="NA1:NE1"/>
-    <mergeCell ref="NF1:NJ1"/>
-    <mergeCell ref="NK1:NO1"/>
-    <mergeCell ref="LR1:LV1"/>
-    <mergeCell ref="LW1:MA1"/>
-    <mergeCell ref="MB1:MF1"/>
-    <mergeCell ref="MG1:MK1"/>
-    <mergeCell ref="ML1:MP1"/>
-    <mergeCell ref="MQ1:MU1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2312,11 +2318,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8527676C-36D2-453A-A1D5-2B015A45A75A}">
-  <dimension ref="A1:NT52"/>
+  <dimension ref="A1:NT53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16:D19"/>
+      <selection pane="bottomLeft" activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -2365,20 +2371,20 @@
       <c r="I1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="51">
+      <c r="J1" s="50">
         <v>45100</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51">
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50">
         <v>45198</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
       <c r="T1" s="52" t="s">
         <v>47</v>
       </c>
@@ -2386,448 +2392,448 @@
       <c r="V1" s="52"/>
       <c r="W1" s="52"/>
       <c r="X1" s="52"/>
-      <c r="Y1" s="51">
+      <c r="Y1" s="50">
         <v>45205</v>
       </c>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51">
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50">
         <v>45206</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="50">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="51">
         <v>45212</v>
       </c>
-      <c r="AJ1" s="50"/>
-      <c r="AK1" s="50"/>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="50">
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51">
         <v>45213</v>
       </c>
-      <c r="AO1" s="50"/>
-      <c r="AP1" s="50"/>
-      <c r="AQ1" s="50"/>
-      <c r="AR1" s="50"/>
-      <c r="AS1" s="51">
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="50">
         <v>45219</v>
       </c>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
-      <c r="AW1" s="51"/>
-      <c r="AX1" s="51">
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="50"/>
+      <c r="AX1" s="50">
         <v>45220</v>
       </c>
-      <c r="AY1" s="51"/>
-      <c r="AZ1" s="51"/>
-      <c r="BA1" s="51"/>
-      <c r="BB1" s="51"/>
-      <c r="BC1" s="51">
+      <c r="AY1" s="50"/>
+      <c r="AZ1" s="50"/>
+      <c r="BA1" s="50"/>
+      <c r="BB1" s="50"/>
+      <c r="BC1" s="50">
         <v>45226</v>
       </c>
-      <c r="BD1" s="51"/>
-      <c r="BE1" s="51"/>
-      <c r="BF1" s="51"/>
-      <c r="BG1" s="51"/>
-      <c r="BH1" s="51">
+      <c r="BD1" s="50"/>
+      <c r="BE1" s="50"/>
+      <c r="BF1" s="50"/>
+      <c r="BG1" s="50"/>
+      <c r="BH1" s="50">
         <v>45227</v>
       </c>
-      <c r="BI1" s="51"/>
-      <c r="BJ1" s="51"/>
-      <c r="BK1" s="51"/>
-      <c r="BL1" s="51"/>
-      <c r="BM1" s="51">
+      <c r="BI1" s="50"/>
+      <c r="BJ1" s="50"/>
+      <c r="BK1" s="50"/>
+      <c r="BL1" s="50"/>
+      <c r="BM1" s="50">
         <v>45233</v>
       </c>
-      <c r="BN1" s="51"/>
-      <c r="BO1" s="51"/>
-      <c r="BP1" s="51"/>
-      <c r="BQ1" s="51"/>
-      <c r="BR1" s="51">
+      <c r="BN1" s="50"/>
+      <c r="BO1" s="50"/>
+      <c r="BP1" s="50"/>
+      <c r="BQ1" s="50"/>
+      <c r="BR1" s="50">
         <v>45234</v>
       </c>
-      <c r="BS1" s="51"/>
-      <c r="BT1" s="51"/>
-      <c r="BU1" s="51"/>
-      <c r="BV1" s="51"/>
-      <c r="BW1" s="51">
+      <c r="BS1" s="50"/>
+      <c r="BT1" s="50"/>
+      <c r="BU1" s="50"/>
+      <c r="BV1" s="50"/>
+      <c r="BW1" s="50">
         <v>45240</v>
       </c>
-      <c r="BX1" s="51"/>
-      <c r="BY1" s="51"/>
-      <c r="BZ1" s="51"/>
-      <c r="CA1" s="51"/>
-      <c r="CB1" s="51">
+      <c r="BX1" s="50"/>
+      <c r="BY1" s="50"/>
+      <c r="BZ1" s="50"/>
+      <c r="CA1" s="50"/>
+      <c r="CB1" s="50">
         <v>45241</v>
       </c>
-      <c r="CC1" s="51"/>
-      <c r="CD1" s="51"/>
-      <c r="CE1" s="51"/>
-      <c r="CF1" s="51"/>
-      <c r="CG1" s="51">
+      <c r="CC1" s="50"/>
+      <c r="CD1" s="50"/>
+      <c r="CE1" s="50"/>
+      <c r="CF1" s="50"/>
+      <c r="CG1" s="50">
         <v>45247</v>
       </c>
-      <c r="CH1" s="51"/>
-      <c r="CI1" s="51"/>
-      <c r="CJ1" s="51"/>
-      <c r="CK1" s="51"/>
-      <c r="CL1" s="51">
+      <c r="CH1" s="50"/>
+      <c r="CI1" s="50"/>
+      <c r="CJ1" s="50"/>
+      <c r="CK1" s="50"/>
+      <c r="CL1" s="50">
         <v>45248</v>
       </c>
-      <c r="CM1" s="51"/>
-      <c r="CN1" s="51"/>
-      <c r="CO1" s="51"/>
-      <c r="CP1" s="51"/>
-      <c r="CQ1" s="51">
+      <c r="CM1" s="50"/>
+      <c r="CN1" s="50"/>
+      <c r="CO1" s="50"/>
+      <c r="CP1" s="50"/>
+      <c r="CQ1" s="50">
         <v>45254</v>
       </c>
-      <c r="CR1" s="51"/>
-      <c r="CS1" s="51"/>
-      <c r="CT1" s="51"/>
-      <c r="CU1" s="51"/>
-      <c r="CV1" s="51">
+      <c r="CR1" s="50"/>
+      <c r="CS1" s="50"/>
+      <c r="CT1" s="50"/>
+      <c r="CU1" s="50"/>
+      <c r="CV1" s="50">
         <v>45255</v>
       </c>
-      <c r="CW1" s="51"/>
-      <c r="CX1" s="51"/>
-      <c r="CY1" s="51"/>
-      <c r="CZ1" s="51"/>
-      <c r="DA1" s="51">
+      <c r="CW1" s="50"/>
+      <c r="CX1" s="50"/>
+      <c r="CY1" s="50"/>
+      <c r="CZ1" s="50"/>
+      <c r="DA1" s="50">
         <v>45261</v>
       </c>
-      <c r="DB1" s="51"/>
-      <c r="DC1" s="51"/>
-      <c r="DD1" s="51"/>
-      <c r="DE1" s="51"/>
-      <c r="DF1" s="51">
+      <c r="DB1" s="50"/>
+      <c r="DC1" s="50"/>
+      <c r="DD1" s="50"/>
+      <c r="DE1" s="50"/>
+      <c r="DF1" s="50">
         <v>45262</v>
       </c>
-      <c r="DG1" s="51"/>
-      <c r="DH1" s="51"/>
-      <c r="DI1" s="51"/>
-      <c r="DJ1" s="51"/>
-      <c r="DK1" s="51">
+      <c r="DG1" s="50"/>
+      <c r="DH1" s="50"/>
+      <c r="DI1" s="50"/>
+      <c r="DJ1" s="50"/>
+      <c r="DK1" s="50">
         <v>45268</v>
       </c>
-      <c r="DL1" s="51"/>
-      <c r="DM1" s="51"/>
-      <c r="DN1" s="51"/>
-      <c r="DO1" s="51"/>
-      <c r="DP1" s="51">
+      <c r="DL1" s="50"/>
+      <c r="DM1" s="50"/>
+      <c r="DN1" s="50"/>
+      <c r="DO1" s="50"/>
+      <c r="DP1" s="50">
         <v>45269</v>
       </c>
-      <c r="DQ1" s="51"/>
-      <c r="DR1" s="51"/>
-      <c r="DS1" s="51"/>
-      <c r="DT1" s="51"/>
-      <c r="DU1" s="51">
+      <c r="DQ1" s="50"/>
+      <c r="DR1" s="50"/>
+      <c r="DS1" s="50"/>
+      <c r="DT1" s="50"/>
+      <c r="DU1" s="50">
         <v>45275</v>
       </c>
-      <c r="DV1" s="51"/>
-      <c r="DW1" s="51"/>
-      <c r="DX1" s="51"/>
-      <c r="DY1" s="51"/>
-      <c r="DZ1" s="51">
+      <c r="DV1" s="50"/>
+      <c r="DW1" s="50"/>
+      <c r="DX1" s="50"/>
+      <c r="DY1" s="50"/>
+      <c r="DZ1" s="50">
         <v>45276</v>
       </c>
-      <c r="EA1" s="51"/>
-      <c r="EB1" s="51"/>
-      <c r="EC1" s="51"/>
-      <c r="ED1" s="51"/>
-      <c r="EE1" s="50">
+      <c r="EA1" s="50"/>
+      <c r="EB1" s="50"/>
+      <c r="EC1" s="50"/>
+      <c r="ED1" s="50"/>
+      <c r="EE1" s="51">
         <v>45282</v>
       </c>
-      <c r="EF1" s="50"/>
-      <c r="EG1" s="50"/>
-      <c r="EH1" s="50"/>
-      <c r="EI1" s="50"/>
-      <c r="EJ1" s="50">
+      <c r="EF1" s="51"/>
+      <c r="EG1" s="51"/>
+      <c r="EH1" s="51"/>
+      <c r="EI1" s="51"/>
+      <c r="EJ1" s="51">
         <v>45283</v>
       </c>
-      <c r="EK1" s="50"/>
-      <c r="EL1" s="50"/>
-      <c r="EM1" s="50"/>
-      <c r="EN1" s="50"/>
-      <c r="EO1" s="50">
+      <c r="EK1" s="51"/>
+      <c r="EL1" s="51"/>
+      <c r="EM1" s="51"/>
+      <c r="EN1" s="51"/>
+      <c r="EO1" s="51">
         <v>45289</v>
       </c>
-      <c r="EP1" s="50"/>
-      <c r="EQ1" s="50"/>
-      <c r="ER1" s="50"/>
-      <c r="ES1" s="50"/>
-      <c r="ET1" s="50">
+      <c r="EP1" s="51"/>
+      <c r="EQ1" s="51"/>
+      <c r="ER1" s="51"/>
+      <c r="ES1" s="51"/>
+      <c r="ET1" s="51">
         <v>45290</v>
       </c>
-      <c r="EU1" s="50"/>
-      <c r="EV1" s="50"/>
-      <c r="EW1" s="50"/>
-      <c r="EX1" s="50"/>
-      <c r="EY1" s="51">
+      <c r="EU1" s="51"/>
+      <c r="EV1" s="51"/>
+      <c r="EW1" s="51"/>
+      <c r="EX1" s="51"/>
+      <c r="EY1" s="50">
         <v>45296</v>
       </c>
-      <c r="EZ1" s="51"/>
-      <c r="FA1" s="51"/>
-      <c r="FB1" s="51"/>
-      <c r="FC1" s="51"/>
-      <c r="FD1" s="51">
+      <c r="EZ1" s="50"/>
+      <c r="FA1" s="50"/>
+      <c r="FB1" s="50"/>
+      <c r="FC1" s="50"/>
+      <c r="FD1" s="50">
         <v>45297</v>
       </c>
-      <c r="FE1" s="51"/>
-      <c r="FF1" s="51"/>
-      <c r="FG1" s="51"/>
-      <c r="FH1" s="51"/>
-      <c r="FI1" s="51">
+      <c r="FE1" s="50"/>
+      <c r="FF1" s="50"/>
+      <c r="FG1" s="50"/>
+      <c r="FH1" s="50"/>
+      <c r="FI1" s="50">
         <v>45303</v>
       </c>
-      <c r="FJ1" s="51"/>
-      <c r="FK1" s="51"/>
-      <c r="FL1" s="51"/>
-      <c r="FM1" s="51"/>
-      <c r="FN1" s="51">
+      <c r="FJ1" s="50"/>
+      <c r="FK1" s="50"/>
+      <c r="FL1" s="50"/>
+      <c r="FM1" s="50"/>
+      <c r="FN1" s="50">
         <v>45304</v>
       </c>
-      <c r="FO1" s="51"/>
-      <c r="FP1" s="51"/>
-      <c r="FQ1" s="51"/>
-      <c r="FR1" s="51"/>
-      <c r="FS1" s="51">
+      <c r="FO1" s="50"/>
+      <c r="FP1" s="50"/>
+      <c r="FQ1" s="50"/>
+      <c r="FR1" s="50"/>
+      <c r="FS1" s="50">
         <v>45310</v>
       </c>
-      <c r="FT1" s="51"/>
-      <c r="FU1" s="51"/>
-      <c r="FV1" s="51"/>
-      <c r="FW1" s="51"/>
-      <c r="FX1" s="51">
+      <c r="FT1" s="50"/>
+      <c r="FU1" s="50"/>
+      <c r="FV1" s="50"/>
+      <c r="FW1" s="50"/>
+      <c r="FX1" s="50">
         <v>45311</v>
       </c>
-      <c r="FY1" s="51"/>
-      <c r="FZ1" s="51"/>
-      <c r="GA1" s="51"/>
-      <c r="GB1" s="51"/>
-      <c r="GC1" s="51">
+      <c r="FY1" s="50"/>
+      <c r="FZ1" s="50"/>
+      <c r="GA1" s="50"/>
+      <c r="GB1" s="50"/>
+      <c r="GC1" s="50">
         <v>45317</v>
       </c>
-      <c r="GD1" s="51"/>
-      <c r="GE1" s="51"/>
-      <c r="GF1" s="51"/>
-      <c r="GG1" s="51"/>
-      <c r="GH1" s="51">
+      <c r="GD1" s="50"/>
+      <c r="GE1" s="50"/>
+      <c r="GF1" s="50"/>
+      <c r="GG1" s="50"/>
+      <c r="GH1" s="50">
         <v>45318</v>
       </c>
-      <c r="GI1" s="51"/>
-      <c r="GJ1" s="51"/>
-      <c r="GK1" s="51"/>
-      <c r="GL1" s="51"/>
-      <c r="GM1" s="51">
+      <c r="GI1" s="50"/>
+      <c r="GJ1" s="50"/>
+      <c r="GK1" s="50"/>
+      <c r="GL1" s="50"/>
+      <c r="GM1" s="50">
         <v>45324</v>
       </c>
-      <c r="GN1" s="51"/>
-      <c r="GO1" s="51"/>
-      <c r="GP1" s="51"/>
-      <c r="GQ1" s="51"/>
-      <c r="GR1" s="51">
+      <c r="GN1" s="50"/>
+      <c r="GO1" s="50"/>
+      <c r="GP1" s="50"/>
+      <c r="GQ1" s="50"/>
+      <c r="GR1" s="50">
         <v>45325</v>
       </c>
-      <c r="GS1" s="51"/>
-      <c r="GT1" s="51"/>
-      <c r="GU1" s="51"/>
-      <c r="GV1" s="51"/>
-      <c r="GW1" s="51">
+      <c r="GS1" s="50"/>
+      <c r="GT1" s="50"/>
+      <c r="GU1" s="50"/>
+      <c r="GV1" s="50"/>
+      <c r="GW1" s="50">
         <v>45331</v>
       </c>
-      <c r="GX1" s="51"/>
-      <c r="GY1" s="51"/>
-      <c r="GZ1" s="51"/>
-      <c r="HA1" s="51"/>
-      <c r="HB1" s="51">
+      <c r="GX1" s="50"/>
+      <c r="GY1" s="50"/>
+      <c r="GZ1" s="50"/>
+      <c r="HA1" s="50"/>
+      <c r="HB1" s="50">
         <v>45332</v>
       </c>
-      <c r="HC1" s="51"/>
-      <c r="HD1" s="51"/>
-      <c r="HE1" s="51"/>
-      <c r="HF1" s="51"/>
-      <c r="HG1" s="51">
+      <c r="HC1" s="50"/>
+      <c r="HD1" s="50"/>
+      <c r="HE1" s="50"/>
+      <c r="HF1" s="50"/>
+      <c r="HG1" s="50">
         <v>45338</v>
       </c>
-      <c r="HH1" s="51"/>
-      <c r="HI1" s="51"/>
-      <c r="HJ1" s="51"/>
-      <c r="HK1" s="51"/>
-      <c r="HL1" s="51">
+      <c r="HH1" s="50"/>
+      <c r="HI1" s="50"/>
+      <c r="HJ1" s="50"/>
+      <c r="HK1" s="50"/>
+      <c r="HL1" s="50">
         <v>45339</v>
       </c>
-      <c r="HM1" s="51"/>
-      <c r="HN1" s="51"/>
-      <c r="HO1" s="51"/>
-      <c r="HP1" s="51"/>
-      <c r="HQ1" s="51">
+      <c r="HM1" s="50"/>
+      <c r="HN1" s="50"/>
+      <c r="HO1" s="50"/>
+      <c r="HP1" s="50"/>
+      <c r="HQ1" s="50">
         <v>45345</v>
       </c>
-      <c r="HR1" s="51"/>
-      <c r="HS1" s="51"/>
-      <c r="HT1" s="51"/>
-      <c r="HU1" s="51"/>
-      <c r="HV1" s="51"/>
-      <c r="HW1" s="51"/>
-      <c r="HX1" s="51"/>
-      <c r="HY1" s="51"/>
-      <c r="HZ1" s="51"/>
-      <c r="IA1" s="51"/>
-      <c r="IB1" s="51"/>
-      <c r="IC1" s="51"/>
-      <c r="ID1" s="51"/>
-      <c r="IE1" s="51"/>
-      <c r="IF1" s="51"/>
-      <c r="IG1" s="51"/>
-      <c r="IH1" s="51"/>
-      <c r="II1" s="51"/>
-      <c r="IJ1" s="51"/>
-      <c r="IK1" s="51"/>
-      <c r="IL1" s="51"/>
-      <c r="IM1" s="51"/>
-      <c r="IN1" s="51"/>
-      <c r="IO1" s="51"/>
-      <c r="IP1" s="51"/>
-      <c r="IQ1" s="51"/>
-      <c r="IR1" s="51"/>
-      <c r="IS1" s="51"/>
-      <c r="IT1" s="51"/>
-      <c r="IU1" s="51"/>
-      <c r="IV1" s="51"/>
-      <c r="IW1" s="51"/>
-      <c r="IX1" s="51"/>
-      <c r="IY1" s="51"/>
-      <c r="IZ1" s="51"/>
-      <c r="JA1" s="51"/>
-      <c r="JB1" s="51"/>
-      <c r="JC1" s="51"/>
-      <c r="JD1" s="51"/>
-      <c r="JE1" s="51"/>
-      <c r="JF1" s="51"/>
-      <c r="JG1" s="51"/>
-      <c r="JH1" s="51"/>
-      <c r="JI1" s="51"/>
-      <c r="JJ1" s="51"/>
-      <c r="JK1" s="51"/>
-      <c r="JL1" s="51"/>
-      <c r="JM1" s="51"/>
-      <c r="JN1" s="51"/>
-      <c r="JO1" s="51"/>
-      <c r="JP1" s="51"/>
-      <c r="JQ1" s="51"/>
-      <c r="JR1" s="51"/>
-      <c r="JS1" s="51"/>
-      <c r="JT1" s="51"/>
-      <c r="JU1" s="51"/>
-      <c r="JV1" s="51"/>
-      <c r="JW1" s="51"/>
-      <c r="JX1" s="51"/>
-      <c r="JY1" s="51"/>
-      <c r="JZ1" s="51"/>
-      <c r="KA1" s="51"/>
-      <c r="KB1" s="51"/>
-      <c r="KC1" s="51"/>
-      <c r="KD1" s="51"/>
-      <c r="KE1" s="51"/>
-      <c r="KF1" s="51"/>
-      <c r="KG1" s="51"/>
-      <c r="KH1" s="51"/>
-      <c r="KI1" s="51"/>
-      <c r="KJ1" s="51"/>
-      <c r="KK1" s="51"/>
-      <c r="KL1" s="51"/>
-      <c r="KM1" s="51"/>
-      <c r="KN1" s="51"/>
-      <c r="KO1" s="51"/>
-      <c r="KP1" s="51"/>
-      <c r="KQ1" s="51"/>
-      <c r="KR1" s="51"/>
-      <c r="KS1" s="51"/>
-      <c r="KT1" s="51"/>
-      <c r="KU1" s="51"/>
-      <c r="KV1" s="51"/>
-      <c r="KW1" s="51"/>
-      <c r="KX1" s="51"/>
-      <c r="KY1" s="51"/>
-      <c r="KZ1" s="51"/>
-      <c r="LA1" s="51"/>
-      <c r="LB1" s="51"/>
-      <c r="LC1" s="51"/>
-      <c r="LD1" s="51"/>
-      <c r="LE1" s="51"/>
-      <c r="LF1" s="51"/>
-      <c r="LG1" s="51"/>
-      <c r="LH1" s="51"/>
-      <c r="LI1" s="51"/>
-      <c r="LJ1" s="51"/>
-      <c r="LK1" s="51"/>
-      <c r="LL1" s="51"/>
-      <c r="LM1" s="51"/>
-      <c r="LN1" s="51"/>
-      <c r="LO1" s="51"/>
-      <c r="LP1" s="51"/>
-      <c r="LQ1" s="51"/>
-      <c r="LR1" s="51"/>
-      <c r="LS1" s="51"/>
-      <c r="LT1" s="51"/>
-      <c r="LU1" s="51"/>
-      <c r="LV1" s="51"/>
-      <c r="LW1" s="51"/>
-      <c r="LX1" s="51"/>
-      <c r="LY1" s="51"/>
-      <c r="LZ1" s="51"/>
-      <c r="MA1" s="51"/>
-      <c r="MB1" s="51"/>
-      <c r="MC1" s="51"/>
-      <c r="MD1" s="51"/>
-      <c r="ME1" s="51"/>
-      <c r="MF1" s="51"/>
-      <c r="MG1" s="51"/>
-      <c r="MH1" s="51"/>
-      <c r="MI1" s="51"/>
-      <c r="MJ1" s="51"/>
-      <c r="MK1" s="51"/>
-      <c r="ML1" s="51"/>
-      <c r="MM1" s="51"/>
-      <c r="MN1" s="51"/>
-      <c r="MO1" s="51"/>
-      <c r="MP1" s="51"/>
-      <c r="MQ1" s="51"/>
-      <c r="MR1" s="51"/>
-      <c r="MS1" s="51"/>
-      <c r="MT1" s="51"/>
-      <c r="MU1" s="51"/>
-      <c r="MV1" s="51"/>
-      <c r="MW1" s="51"/>
-      <c r="MX1" s="51"/>
-      <c r="MY1" s="51"/>
-      <c r="MZ1" s="51"/>
-      <c r="NA1" s="51"/>
-      <c r="NB1" s="51"/>
-      <c r="NC1" s="51"/>
-      <c r="ND1" s="51"/>
-      <c r="NE1" s="51"/>
-      <c r="NF1" s="51"/>
-      <c r="NG1" s="51"/>
-      <c r="NH1" s="51"/>
-      <c r="NI1" s="51"/>
-      <c r="NJ1" s="51"/>
-      <c r="NK1" s="51"/>
-      <c r="NL1" s="51"/>
-      <c r="NM1" s="51"/>
-      <c r="NN1" s="51"/>
-      <c r="NO1" s="51"/>
-      <c r="NP1" s="51"/>
-      <c r="NQ1" s="51"/>
-      <c r="NR1" s="51"/>
-      <c r="NS1" s="51"/>
-      <c r="NT1" s="51"/>
+      <c r="HR1" s="50"/>
+      <c r="HS1" s="50"/>
+      <c r="HT1" s="50"/>
+      <c r="HU1" s="50"/>
+      <c r="HV1" s="50"/>
+      <c r="HW1" s="50"/>
+      <c r="HX1" s="50"/>
+      <c r="HY1" s="50"/>
+      <c r="HZ1" s="50"/>
+      <c r="IA1" s="50"/>
+      <c r="IB1" s="50"/>
+      <c r="IC1" s="50"/>
+      <c r="ID1" s="50"/>
+      <c r="IE1" s="50"/>
+      <c r="IF1" s="50"/>
+      <c r="IG1" s="50"/>
+      <c r="IH1" s="50"/>
+      <c r="II1" s="50"/>
+      <c r="IJ1" s="50"/>
+      <c r="IK1" s="50"/>
+      <c r="IL1" s="50"/>
+      <c r="IM1" s="50"/>
+      <c r="IN1" s="50"/>
+      <c r="IO1" s="50"/>
+      <c r="IP1" s="50"/>
+      <c r="IQ1" s="50"/>
+      <c r="IR1" s="50"/>
+      <c r="IS1" s="50"/>
+      <c r="IT1" s="50"/>
+      <c r="IU1" s="50"/>
+      <c r="IV1" s="50"/>
+      <c r="IW1" s="50"/>
+      <c r="IX1" s="50"/>
+      <c r="IY1" s="50"/>
+      <c r="IZ1" s="50"/>
+      <c r="JA1" s="50"/>
+      <c r="JB1" s="50"/>
+      <c r="JC1" s="50"/>
+      <c r="JD1" s="50"/>
+      <c r="JE1" s="50"/>
+      <c r="JF1" s="50"/>
+      <c r="JG1" s="50"/>
+      <c r="JH1" s="50"/>
+      <c r="JI1" s="50"/>
+      <c r="JJ1" s="50"/>
+      <c r="JK1" s="50"/>
+      <c r="JL1" s="50"/>
+      <c r="JM1" s="50"/>
+      <c r="JN1" s="50"/>
+      <c r="JO1" s="50"/>
+      <c r="JP1" s="50"/>
+      <c r="JQ1" s="50"/>
+      <c r="JR1" s="50"/>
+      <c r="JS1" s="50"/>
+      <c r="JT1" s="50"/>
+      <c r="JU1" s="50"/>
+      <c r="JV1" s="50"/>
+      <c r="JW1" s="50"/>
+      <c r="JX1" s="50"/>
+      <c r="JY1" s="50"/>
+      <c r="JZ1" s="50"/>
+      <c r="KA1" s="50"/>
+      <c r="KB1" s="50"/>
+      <c r="KC1" s="50"/>
+      <c r="KD1" s="50"/>
+      <c r="KE1" s="50"/>
+      <c r="KF1" s="50"/>
+      <c r="KG1" s="50"/>
+      <c r="KH1" s="50"/>
+      <c r="KI1" s="50"/>
+      <c r="KJ1" s="50"/>
+      <c r="KK1" s="50"/>
+      <c r="KL1" s="50"/>
+      <c r="KM1" s="50"/>
+      <c r="KN1" s="50"/>
+      <c r="KO1" s="50"/>
+      <c r="KP1" s="50"/>
+      <c r="KQ1" s="50"/>
+      <c r="KR1" s="50"/>
+      <c r="KS1" s="50"/>
+      <c r="KT1" s="50"/>
+      <c r="KU1" s="50"/>
+      <c r="KV1" s="50"/>
+      <c r="KW1" s="50"/>
+      <c r="KX1" s="50"/>
+      <c r="KY1" s="50"/>
+      <c r="KZ1" s="50"/>
+      <c r="LA1" s="50"/>
+      <c r="LB1" s="50"/>
+      <c r="LC1" s="50"/>
+      <c r="LD1" s="50"/>
+      <c r="LE1" s="50"/>
+      <c r="LF1" s="50"/>
+      <c r="LG1" s="50"/>
+      <c r="LH1" s="50"/>
+      <c r="LI1" s="50"/>
+      <c r="LJ1" s="50"/>
+      <c r="LK1" s="50"/>
+      <c r="LL1" s="50"/>
+      <c r="LM1" s="50"/>
+      <c r="LN1" s="50"/>
+      <c r="LO1" s="50"/>
+      <c r="LP1" s="50"/>
+      <c r="LQ1" s="50"/>
+      <c r="LR1" s="50"/>
+      <c r="LS1" s="50"/>
+      <c r="LT1" s="50"/>
+      <c r="LU1" s="50"/>
+      <c r="LV1" s="50"/>
+      <c r="LW1" s="50"/>
+      <c r="LX1" s="50"/>
+      <c r="LY1" s="50"/>
+      <c r="LZ1" s="50"/>
+      <c r="MA1" s="50"/>
+      <c r="MB1" s="50"/>
+      <c r="MC1" s="50"/>
+      <c r="MD1" s="50"/>
+      <c r="ME1" s="50"/>
+      <c r="MF1" s="50"/>
+      <c r="MG1" s="50"/>
+      <c r="MH1" s="50"/>
+      <c r="MI1" s="50"/>
+      <c r="MJ1" s="50"/>
+      <c r="MK1" s="50"/>
+      <c r="ML1" s="50"/>
+      <c r="MM1" s="50"/>
+      <c r="MN1" s="50"/>
+      <c r="MO1" s="50"/>
+      <c r="MP1" s="50"/>
+      <c r="MQ1" s="50"/>
+      <c r="MR1" s="50"/>
+      <c r="MS1" s="50"/>
+      <c r="MT1" s="50"/>
+      <c r="MU1" s="50"/>
+      <c r="MV1" s="50"/>
+      <c r="MW1" s="50"/>
+      <c r="MX1" s="50"/>
+      <c r="MY1" s="50"/>
+      <c r="MZ1" s="50"/>
+      <c r="NA1" s="50"/>
+      <c r="NB1" s="50"/>
+      <c r="NC1" s="50"/>
+      <c r="ND1" s="50"/>
+      <c r="NE1" s="50"/>
+      <c r="NF1" s="50"/>
+      <c r="NG1" s="50"/>
+      <c r="NH1" s="50"/>
+      <c r="NI1" s="50"/>
+      <c r="NJ1" s="50"/>
+      <c r="NK1" s="50"/>
+      <c r="NL1" s="50"/>
+      <c r="NM1" s="50"/>
+      <c r="NN1" s="50"/>
+      <c r="NO1" s="50"/>
+      <c r="NP1" s="50"/>
+      <c r="NQ1" s="50"/>
+      <c r="NR1" s="50"/>
+      <c r="NS1" s="50"/>
+      <c r="NT1" s="50"/>
     </row>
     <row r="2" spans="1:384" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -2847,12 +2853,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="31">
-        <f>C2/($C$52/100)</f>
-        <v>2.9069767441860463</v>
+        <f>C2/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G2" s="31">
-        <f>D2/($D$52/100)</f>
-        <v>30.769230769230766</v>
+        <f>D2/($D$53/100)</f>
+        <v>16.326530612244898</v>
       </c>
       <c r="H2" s="20">
         <f>IF(MIN(H3:H6)=0,"-",MIN(H3:H6))</f>
@@ -2887,16 +2893,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="42">
-        <f t="shared" ref="E3:E49" si="0">IF(C3-D3=C3,0,C3-D3)</f>
+        <f t="shared" ref="E3:E50" si="0">IF(C3-D3=C3,0,C3-D3)</f>
         <v>0.5</v>
       </c>
       <c r="F3" s="32">
-        <f t="shared" ref="F3:F27" si="1">C3/($C$52/100)</f>
-        <v>0.87209302325581395</v>
+        <f>C3/($C$53/100)</f>
+        <v>0.86705202312138729</v>
       </c>
       <c r="G3" s="32">
-        <f t="shared" ref="G3:G52" si="2">D3/($D$52/100)</f>
-        <v>7.6923076923076916</v>
+        <f>D3/($D$53/100)</f>
+        <v>4.0816326530612246</v>
       </c>
       <c r="H3" s="18">
         <v>45198</v>
@@ -2924,12 +2930,12 @@
         <v>-0.5</v>
       </c>
       <c r="F4" s="32">
-        <f t="shared" si="1"/>
-        <v>0.58139534883720934</v>
+        <f>C4/($C$53/100)</f>
+        <v>0.5780346820809249</v>
       </c>
       <c r="G4" s="32">
-        <f t="shared" si="2"/>
-        <v>11.538461538461538</v>
+        <f>D4/($D$53/100)</f>
+        <v>6.1224489795918364</v>
       </c>
       <c r="H4" s="18">
         <v>45198</v>
@@ -2960,12 +2966,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="32">
-        <f t="shared" si="1"/>
-        <v>0.29069767441860467</v>
+        <f>C5/($C$53/100)</f>
+        <v>0.28901734104046245</v>
       </c>
       <c r="G5" s="32">
-        <f t="shared" si="2"/>
-        <v>3.8461538461538458</v>
+        <f>D5/($D$53/100)</f>
+        <v>2.0408163265306123</v>
       </c>
       <c r="H5" s="18">
         <v>45198</v>
@@ -2993,12 +2999,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="32">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744187</v>
+        <f>C6/($C$53/100)</f>
+        <v>1.1560693641618498</v>
       </c>
       <c r="G6" s="32">
-        <f t="shared" si="2"/>
-        <v>7.6923076923076916</v>
+        <f>D6/($D$53/100)</f>
+        <v>4.0816326530612246</v>
       </c>
       <c r="H6" s="18">
         <v>45198</v>
@@ -3029,12 +3035,12 @@
         <v>7</v>
       </c>
       <c r="F7" s="31">
-        <f t="shared" si="1"/>
-        <v>9.3023255813953494</v>
+        <f>C7/($C$53/100)</f>
+        <v>9.2485549132947984</v>
       </c>
       <c r="G7" s="31">
-        <f t="shared" si="2"/>
-        <v>69.230769230769226</v>
+        <f>D7/($D$53/100)</f>
+        <v>36.734693877551024</v>
       </c>
       <c r="H7" s="20">
         <f>IF(MIN(H8:H14)=0,"-",MIN(H8:H14))</f>
@@ -3096,12 +3102,12 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="32">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744187</v>
+        <f>C8/($C$53/100)</f>
+        <v>1.1560693641618498</v>
       </c>
       <c r="G8" s="32">
-        <f t="shared" si="2"/>
-        <v>11.538461538461538</v>
+        <f>D8/($D$53/100)</f>
+        <v>6.1224489795918364</v>
       </c>
       <c r="H8" s="18">
         <v>45205</v>
@@ -3133,12 +3139,12 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="32">
-        <f t="shared" si="1"/>
-        <v>0.58139534883720934</v>
+        <f>C9/($C$53/100)</f>
+        <v>0.5780346820809249</v>
       </c>
       <c r="G9" s="32">
-        <f t="shared" si="2"/>
-        <v>3.8461538461538458</v>
+        <f>D9/($D$53/100)</f>
+        <v>2.0408163265306123</v>
       </c>
       <c r="H9" s="18">
         <v>45205</v>
@@ -3166,12 +3172,12 @@
         <v>1.5</v>
       </c>
       <c r="F10" s="32">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744187</v>
+        <f>C10/($C$53/100)</f>
+        <v>1.1560693641618498</v>
       </c>
       <c r="G10" s="32">
-        <f t="shared" si="2"/>
-        <v>3.8461538461538458</v>
+        <f>D10/($D$53/100)</f>
+        <v>2.0408163265306123</v>
       </c>
       <c r="H10" s="18">
         <v>45205</v>
@@ -3200,12 +3206,12 @@
         <v>0</v>
       </c>
       <c r="F11" s="32">
-        <f t="shared" si="1"/>
-        <v>0.58139534883720934</v>
+        <f>C11/($C$53/100)</f>
+        <v>0.5780346820809249</v>
       </c>
       <c r="G11" s="32">
-        <f t="shared" si="2"/>
-        <v>7.6923076923076916</v>
+        <f>D11/($D$53/100)</f>
+        <v>4.0816326530612246</v>
       </c>
       <c r="H11" s="18">
         <v>45205</v>
@@ -3236,12 +3242,12 @@
         <v>3.5</v>
       </c>
       <c r="F12" s="32">
-        <f t="shared" si="1"/>
-        <v>2.3255813953488373</v>
+        <f>C12/($C$53/100)</f>
+        <v>2.3121387283236996</v>
       </c>
       <c r="G12" s="32">
-        <f t="shared" si="2"/>
-        <v>3.8461538461538458</v>
+        <f>D12/($D$53/100)</f>
+        <v>2.0408163265306123</v>
       </c>
       <c r="H12" s="18">
         <v>45206</v>
@@ -3272,12 +3278,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="32">
-        <f t="shared" si="1"/>
-        <v>1.7441860465116279</v>
+        <f>C13/($C$53/100)</f>
+        <v>1.7341040462427746</v>
       </c>
       <c r="G13" s="32">
-        <f t="shared" si="2"/>
-        <v>7.6923076923076916</v>
+        <f>D13/($D$53/100)</f>
+        <v>4.0816326530612246</v>
       </c>
       <c r="H13" s="18">
         <v>45206</v>
@@ -3307,12 +3313,12 @@
         <v>-1</v>
       </c>
       <c r="F14" s="32">
-        <f t="shared" si="1"/>
-        <v>1.7441860465116279</v>
+        <f>C14/($C$53/100)</f>
+        <v>1.7341040462427746</v>
       </c>
       <c r="G14" s="32">
-        <f t="shared" si="2"/>
-        <v>30.769230769230766</v>
+        <f>D14/($D$53/100)</f>
+        <v>16.326530612244898</v>
       </c>
       <c r="H14" s="18">
         <v>45206</v>
@@ -3340,38 +3346,59 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="25">
-        <f>SUM(C16:C19)</f>
-        <v>5</v>
+        <f>SUM(C16:C20)</f>
+        <v>6</v>
       </c>
       <c r="D15" s="25">
-        <f>SUM(D16:D19)</f>
-        <v>0</v>
+        <f>SUM(D16:D20)</f>
+        <v>5.5</v>
       </c>
       <c r="E15" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(C15-D15=C15,0,C15-D15)</f>
+        <v>0.5</v>
       </c>
       <c r="F15" s="31">
-        <f t="shared" si="1"/>
-        <v>2.9069767441860463</v>
+        <f>C15/($C$53/100)</f>
+        <v>3.4682080924855492</v>
       </c>
       <c r="G15" s="31">
-        <f>D15/($D$52/100)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="20" t="str">
-        <f>IF(MIN(H16:H19)=0,"-",MIN(H16:H19))</f>
-        <v>-</v>
-      </c>
-      <c r="I15" s="20" t="str">
-        <f>IF(MAX(I16:I19)=0,"-",MAX(I16:I19))</f>
-        <v>-</v>
+        <f>D15/($D$53/100)</f>
+        <v>22.448979591836736</v>
+      </c>
+      <c r="H15" s="20">
+        <f>IF(MIN(H16:H20)=0,"-",MIN(H16:H20))</f>
+        <v>45220</v>
+      </c>
+      <c r="I15" s="20">
+        <f>IF(MAX(I16:I20)=0,"-",MAX(I16:I20))</f>
+        <v>45240</v>
       </c>
       <c r="AS15" s="13"/>
       <c r="AT15" s="13"/>
       <c r="AU15" s="13"/>
       <c r="AV15" s="13"/>
       <c r="AW15" s="13"/>
+      <c r="AX15" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BW15" s="12" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:384" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
@@ -3380,17 +3407,26 @@
       <c r="C16" s="26">
         <v>2</v>
       </c>
-      <c r="E16" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D16" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="42" t="e">
+        <f>IF(C16-D16=C16,0,C16-D16)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="F16" s="32">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744187</v>
-      </c>
-      <c r="G16" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>C16/($C$53/100)</f>
+        <v>1.1560693641618498</v>
+      </c>
+      <c r="G16" s="32" t="e">
+        <f>D16/($D$53/100)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H16" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="AS16" s="15"/>
       <c r="AT16" s="15"/>
@@ -3402,17 +3438,26 @@
       <c r="C17" s="26">
         <v>2</v>
       </c>
-      <c r="E17" s="42">
+      <c r="D17" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="42" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F17" s="32">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744187</v>
-      </c>
-      <c r="G17" s="32">
-        <f>D17/($D$52/100)</f>
-        <v>0</v>
+        <f>C17/($C$53/100)</f>
+        <v>1.1560693641618498</v>
+      </c>
+      <c r="G17" s="32" t="e">
+        <f>D17/($D$53/100)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="AU17" s="15"/>
       <c r="AV17" s="15"/>
@@ -3424,19 +3469,31 @@
       <c r="C18" s="26">
         <v>0.5</v>
       </c>
+      <c r="D18" s="26">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18" s="32">
-        <f t="shared" si="1"/>
-        <v>0.29069767441860467</v>
+        <f>C18/($C$53/100)</f>
+        <v>0.28901734104046245</v>
       </c>
       <c r="G18" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>D18/($D$53/100)</f>
+        <v>2.0408163265306123</v>
+      </c>
+      <c r="H18" s="18">
+        <v>45220</v>
+      </c>
+      <c r="I18" s="18">
+        <v>45221</v>
       </c>
       <c r="AW18" s="15"/>
+      <c r="AX18" s="12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
@@ -3445,198 +3502,230 @@
       <c r="C19" s="26">
         <v>0.5</v>
       </c>
+      <c r="D19" s="26">
+        <v>1</v>
+      </c>
       <c r="E19" s="42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="F19" s="32">
-        <f t="shared" si="1"/>
-        <v>0.29069767441860467</v>
+        <f>C19/($C$53/100)</f>
+        <v>0.28901734104046245</v>
       </c>
       <c r="G19" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>D19/($D$53/100)</f>
+        <v>4.0816326530612246</v>
+      </c>
+      <c r="H19" s="18">
+        <v>45240</v>
+      </c>
+      <c r="I19" s="18">
+        <v>45240</v>
       </c>
       <c r="AW19" s="15"/>
+      <c r="BW19" s="12" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:164" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="26">
+        <v>1</v>
+      </c>
+      <c r="D20" s="26">
+        <v>4</v>
+      </c>
+      <c r="E20" s="42">
+        <f>IF(C20-D20=C20,0,C20-D20)</f>
+        <v>-3</v>
+      </c>
+      <c r="F20" s="32">
+        <f>C20/($C$53/100)</f>
+        <v>0.5780346820809249</v>
+      </c>
+      <c r="G20" s="32">
+        <f>D20/($D$53/100)</f>
+        <v>16.326530612244898</v>
+      </c>
+      <c r="H20" s="18">
+        <v>45226</v>
+      </c>
+      <c r="I20" s="18">
+        <v>45234</v>
+      </c>
+      <c r="AW20" s="15"/>
+      <c r="BH20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR20" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:164" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="10">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="33">
+        <f>C21/($C$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <f>D21/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
         <v>45219</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="AW20" s="16"/>
-    </row>
-    <row r="21" spans="1:164" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="I21" s="10"/>
+      <c r="AW21" s="16"/>
+    </row>
+    <row r="22" spans="1:164" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="25">
-        <f>SUM(C22:C34)</f>
+      <c r="B22" s="19"/>
+      <c r="C22" s="25">
+        <f>SUM(C23:C35)</f>
         <v>75</v>
       </c>
-      <c r="D21" s="25">
-        <f>SUM(D22:D34)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="41">
+      <c r="D22" s="25">
+        <f>SUM(D23:D35)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="31">
-        <f t="shared" si="1"/>
-        <v>43.604651162790695</v>
-      </c>
-      <c r="G21" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="20" t="str">
-        <f>IF(MIN(H22:H27,H29:H34)=0,"-",MIN(H22:H27,H29:H34))</f>
+      <c r="F22" s="31">
+        <f>C22/($C$53/100)</f>
+        <v>43.352601156069362</v>
+      </c>
+      <c r="G22" s="31">
+        <f>D22/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="20" t="str">
+        <f>IF(MIN(H23:H28,H30:H35)=0,"-",MIN(H23:H28,H30:H35))</f>
         <v>-</v>
       </c>
-      <c r="I21" s="20" t="str">
-        <f>IF(MAX(I22:I27,I29:I34)=0,"-",MAX(I22:I27,I29:I34))</f>
+      <c r="I22" s="20" t="str">
+        <f>IF(MAX(I23:I28,I30:I35)=0,"-",MAX(I23:I28,I30:I35))</f>
         <v>-</v>
       </c>
-      <c r="BA21" s="13"/>
-      <c r="BB21" s="13"/>
-      <c r="BC21" s="13"/>
-      <c r="BD21" s="13"/>
-      <c r="BE21" s="13"/>
-      <c r="BF21" s="13"/>
-      <c r="BG21" s="13"/>
-      <c r="BH21" s="13"/>
-      <c r="BI21" s="13"/>
-      <c r="BJ21" s="13"/>
-      <c r="BK21" s="13"/>
-      <c r="BL21" s="13"/>
-      <c r="BM21" s="13"/>
-      <c r="BN21" s="13"/>
-      <c r="BO21" s="13"/>
-      <c r="BP21" s="13"/>
-      <c r="BQ21" s="13"/>
-      <c r="BR21" s="13"/>
-      <c r="BS21" s="13"/>
-      <c r="BT21" s="13"/>
-      <c r="BU21" s="13"/>
-      <c r="BV21" s="13"/>
-      <c r="BW21" s="13"/>
-      <c r="BX21" s="13"/>
-      <c r="BY21" s="13"/>
-      <c r="BZ21" s="13"/>
-      <c r="CA21" s="13"/>
-      <c r="CB21" s="13"/>
-      <c r="CC21" s="13"/>
-      <c r="CD21" s="13"/>
-      <c r="CE21" s="13"/>
-      <c r="CF21" s="13"/>
-      <c r="CG21" s="13"/>
-      <c r="CH21" s="13"/>
-      <c r="CI21" s="13"/>
-      <c r="CJ21" s="13"/>
-      <c r="CK21" s="13"/>
-      <c r="CL21" s="13"/>
-      <c r="CM21" s="13"/>
-      <c r="CN21" s="13"/>
-      <c r="CO21" s="13"/>
-      <c r="CP21" s="13"/>
-      <c r="CQ21" s="13"/>
-      <c r="CR21" s="13"/>
-      <c r="CS21" s="13"/>
-      <c r="CT21" s="13"/>
-      <c r="CU21" s="13"/>
-      <c r="CV21" s="13"/>
-      <c r="CW21" s="13"/>
-      <c r="CX21" s="13"/>
-      <c r="CY21" s="13"/>
-      <c r="CZ21" s="13"/>
-      <c r="DA21" s="13"/>
-      <c r="DB21" s="13"/>
-      <c r="DC21" s="13"/>
-      <c r="DD21" s="13"/>
-      <c r="DE21" s="13"/>
-      <c r="DF21" s="13"/>
-      <c r="DG21" s="13"/>
-      <c r="DH21" s="13"/>
-      <c r="DI21" s="13"/>
-      <c r="DJ21" s="13"/>
-      <c r="DK21" s="13"/>
-      <c r="DL21" s="13"/>
-      <c r="DM21" s="13"/>
-      <c r="DN21" s="13"/>
-      <c r="DO21" s="13"/>
-      <c r="DP21" s="17"/>
-      <c r="DQ21" s="17"/>
-      <c r="DR21" s="17"/>
-      <c r="DS21" s="17"/>
-      <c r="DT21" s="17"/>
-      <c r="DU21" s="17"/>
-      <c r="DV21" s="17"/>
-      <c r="DW21" s="17"/>
-      <c r="DX21" s="17"/>
-      <c r="DY21" s="17"/>
-      <c r="DZ21" s="17"/>
-      <c r="EA21" s="17"/>
-      <c r="EB21" s="17"/>
-      <c r="EC21" s="17"/>
-      <c r="ED21" s="17"/>
-      <c r="EY21" s="17"/>
-      <c r="EZ21" s="17"/>
-      <c r="FA21" s="17"/>
-      <c r="FB21" s="17"/>
-      <c r="FC21" s="17"/>
-      <c r="FD21" s="17"/>
-      <c r="FE21" s="17"/>
-      <c r="FF21" s="17"/>
-      <c r="FG21" s="17"/>
-      <c r="FH21" s="17"/>
-    </row>
-    <row r="22" spans="1:164" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="26">
-        <v>5</v>
-      </c>
-      <c r="E22" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="32">
-        <f t="shared" si="1"/>
-        <v>2.9069767441860463</v>
-      </c>
-      <c r="G22" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BA22" s="15"/>
-      <c r="BB22" s="15"/>
-      <c r="BC22" s="15"/>
-      <c r="BD22" s="15"/>
-      <c r="BE22" s="15"/>
+      <c r="BA22" s="13"/>
+      <c r="BB22" s="13"/>
+      <c r="BC22" s="13"/>
+      <c r="BD22" s="13"/>
+      <c r="BE22" s="13"/>
+      <c r="BF22" s="13"/>
+      <c r="BG22" s="13"/>
+      <c r="BH22" s="13"/>
+      <c r="BI22" s="13"/>
+      <c r="BJ22" s="13"/>
+      <c r="BK22" s="13"/>
+      <c r="BL22" s="13"/>
+      <c r="BM22" s="13"/>
+      <c r="BN22" s="13"/>
+      <c r="BO22" s="13"/>
+      <c r="BP22" s="13"/>
+      <c r="BQ22" s="13"/>
+      <c r="BR22" s="13"/>
+      <c r="BS22" s="13"/>
+      <c r="BT22" s="13"/>
+      <c r="BU22" s="13"/>
+      <c r="BV22" s="13"/>
+      <c r="BW22" s="13"/>
+      <c r="BX22" s="13"/>
+      <c r="BY22" s="13"/>
+      <c r="BZ22" s="13"/>
+      <c r="CA22" s="13"/>
+      <c r="CB22" s="13"/>
+      <c r="CC22" s="13"/>
+      <c r="CD22" s="13"/>
+      <c r="CE22" s="13"/>
+      <c r="CF22" s="13"/>
+      <c r="CG22" s="13"/>
+      <c r="CH22" s="13"/>
+      <c r="CI22" s="13"/>
+      <c r="CJ22" s="13"/>
+      <c r="CK22" s="13"/>
+      <c r="CL22" s="13"/>
+      <c r="CM22" s="13"/>
+      <c r="CN22" s="13"/>
+      <c r="CO22" s="13"/>
+      <c r="CP22" s="13"/>
+      <c r="CQ22" s="13"/>
+      <c r="CR22" s="13"/>
+      <c r="CS22" s="13"/>
+      <c r="CT22" s="13"/>
+      <c r="CU22" s="13"/>
+      <c r="CV22" s="13"/>
+      <c r="CW22" s="13"/>
+      <c r="CX22" s="13"/>
+      <c r="CY22" s="13"/>
+      <c r="CZ22" s="13"/>
+      <c r="DA22" s="13"/>
+      <c r="DB22" s="13"/>
+      <c r="DC22" s="13"/>
+      <c r="DD22" s="13"/>
+      <c r="DE22" s="13"/>
+      <c r="DF22" s="13"/>
+      <c r="DG22" s="13"/>
+      <c r="DH22" s="13"/>
+      <c r="DI22" s="13"/>
+      <c r="DJ22" s="13"/>
+      <c r="DK22" s="13"/>
+      <c r="DL22" s="13"/>
+      <c r="DM22" s="13"/>
+      <c r="DN22" s="13"/>
+      <c r="DO22" s="13"/>
+      <c r="DP22" s="17"/>
+      <c r="DQ22" s="17"/>
+      <c r="DR22" s="17"/>
+      <c r="DS22" s="17"/>
+      <c r="DT22" s="17"/>
+      <c r="DU22" s="17"/>
+      <c r="DV22" s="17"/>
+      <c r="DW22" s="17"/>
+      <c r="DX22" s="17"/>
+      <c r="DY22" s="17"/>
+      <c r="DZ22" s="17"/>
+      <c r="EA22" s="17"/>
+      <c r="EB22" s="17"/>
+      <c r="EC22" s="17"/>
+      <c r="ED22" s="17"/>
+      <c r="EY22" s="17"/>
+      <c r="EZ22" s="17"/>
+      <c r="FA22" s="17"/>
+      <c r="FB22" s="17"/>
+      <c r="FC22" s="17"/>
+      <c r="FD22" s="17"/>
+      <c r="FE22" s="17"/>
+      <c r="FF22" s="17"/>
+      <c r="FG22" s="17"/>
+      <c r="FH22" s="17"/>
     </row>
     <row r="23" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="26">
         <v>5</v>
@@ -3646,22 +3735,22 @@
         <v>0</v>
       </c>
       <c r="F23" s="32">
-        <f t="shared" si="1"/>
-        <v>2.9069767441860463</v>
+        <f>C23/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G23" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BF23" s="15"/>
-      <c r="BG23" s="15"/>
-      <c r="BH23" s="15"/>
-      <c r="BI23" s="15"/>
-      <c r="BJ23" s="15"/>
+        <f>D23/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BA23" s="15"/>
+      <c r="BB23" s="15"/>
+      <c r="BC23" s="15"/>
+      <c r="BD23" s="15"/>
+      <c r="BE23" s="15"/>
     </row>
     <row r="24" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="26">
         <v>5</v>
@@ -3671,22 +3760,22 @@
         <v>0</v>
       </c>
       <c r="F24" s="32">
-        <f t="shared" si="1"/>
-        <v>2.9069767441860463</v>
+        <f>C24/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G24" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BK24" s="15"/>
-      <c r="BL24" s="15"/>
-      <c r="BM24" s="15"/>
-      <c r="BN24" s="15"/>
-      <c r="BO24" s="15"/>
+        <f>D24/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BF24" s="15"/>
+      <c r="BG24" s="15"/>
+      <c r="BH24" s="15"/>
+      <c r="BI24" s="15"/>
+      <c r="BJ24" s="15"/>
     </row>
     <row r="25" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C25" s="26">
         <v>5</v>
@@ -3696,118 +3785,118 @@
         <v>0</v>
       </c>
       <c r="F25" s="32">
-        <f t="shared" si="1"/>
-        <v>2.9069767441860463</v>
+        <f>C25/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G25" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BP25" s="15"/>
-      <c r="BQ25" s="15"/>
-      <c r="BR25" s="15"/>
-      <c r="BS25" s="15"/>
-      <c r="BT25" s="15"/>
+        <f>D25/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BK25" s="15"/>
+      <c r="BL25" s="15"/>
+      <c r="BM25" s="15"/>
+      <c r="BN25" s="15"/>
+      <c r="BO25" s="15"/>
     </row>
     <row r="26" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C26" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E26" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26" s="32">
-        <f t="shared" si="1"/>
-        <v>1.7441860465116279</v>
+        <f>C26/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G26" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BU26" s="15"/>
-      <c r="BV26" s="15"/>
-      <c r="BW26" s="15"/>
+        <f>D26/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BP26" s="15"/>
+      <c r="BQ26" s="15"/>
+      <c r="BR26" s="15"/>
+      <c r="BS26" s="15"/>
+      <c r="BT26" s="15"/>
     </row>
     <row r="27" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="32">
-        <f t="shared" si="1"/>
-        <v>2.3255813953488373</v>
+        <f>C27/($C$53/100)</f>
+        <v>1.7341040462427746</v>
       </c>
       <c r="G27" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BX27" s="15"/>
-      <c r="BY27" s="15"/>
-      <c r="BZ27" s="15"/>
-      <c r="CA27" s="15"/>
+        <f>D27/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BU27" s="15"/>
+      <c r="BV27" s="15"/>
+      <c r="BW27" s="15"/>
     </row>
     <row r="28" spans="1:164" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="26">
+        <v>4</v>
+      </c>
+      <c r="E28" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
+        <f>C28/($C$53/100)</f>
+        <v>2.3121387283236996</v>
+      </c>
+      <c r="G28" s="32">
+        <f>D28/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BX28" s="15"/>
+      <c r="BY28" s="15"/>
+      <c r="BZ28" s="15"/>
+      <c r="CA28" s="15"/>
+    </row>
+    <row r="29" spans="1:164" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="33">
-        <f>C28/($C$52/100)</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="33">
+        <f>C29/($C$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="33">
+        <f>D29/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
         <v>45240</v>
       </c>
-      <c r="I28" s="10"/>
-      <c r="CA28" s="16"/>
-    </row>
-    <row r="29" spans="1:164" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="26">
-        <v>5</v>
-      </c>
-      <c r="E29" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="32">
-        <f t="shared" ref="F29:F52" si="3">C29/($C$52/100)</f>
-        <v>2.9069767441860463</v>
-      </c>
-      <c r="G29" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CB29" s="15"/>
-      <c r="CC29" s="15"/>
-      <c r="CD29" s="15"/>
-      <c r="CE29" s="15"/>
-      <c r="CF29" s="15"/>
+      <c r="I29" s="10"/>
+      <c r="CA29" s="16"/>
     </row>
     <row r="30" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="26">
         <v>5</v>
@@ -3817,811 +3906,911 @@
         <v>0</v>
       </c>
       <c r="F30" s="32">
-        <f t="shared" si="3"/>
-        <v>2.9069767441860463</v>
+        <f t="shared" ref="F30:F53" si="1">C30/($C$53/100)</f>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G30" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CG30" s="15"/>
-      <c r="CH30" s="15"/>
-      <c r="CI30" s="15"/>
-      <c r="CJ30" s="15"/>
-      <c r="CK30" s="15"/>
+        <f>D30/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="CB30" s="15"/>
+      <c r="CC30" s="15"/>
+      <c r="CD30" s="15"/>
+      <c r="CE30" s="15"/>
+      <c r="CF30" s="15"/>
     </row>
     <row r="31" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="26">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E31" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="32">
-        <f t="shared" si="3"/>
-        <v>5.8139534883720927</v>
+        <f t="shared" si="1"/>
+        <v>2.8901734104046244</v>
       </c>
       <c r="G31" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CL31" s="15"/>
-      <c r="CM31" s="15"/>
-      <c r="CN31" s="15"/>
-      <c r="CO31" s="15"/>
-      <c r="CP31" s="15"/>
-      <c r="CQ31" s="15"/>
-      <c r="CR31" s="15"/>
-      <c r="CS31" s="15"/>
-      <c r="CT31" s="15"/>
-      <c r="CU31" s="15"/>
+        <f>D31/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="CG31" s="15"/>
+      <c r="CH31" s="15"/>
+      <c r="CI31" s="15"/>
+      <c r="CJ31" s="15"/>
+      <c r="CK31" s="15"/>
     </row>
     <row r="32" spans="1:164" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E32" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32" s="32">
-        <f t="shared" si="3"/>
-        <v>1.1627906976744187</v>
+        <f t="shared" si="1"/>
+        <v>5.7803468208092488</v>
       </c>
       <c r="G32" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CV32" s="15"/>
-      <c r="CW32" s="15"/>
+        <f>D32/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="CL32" s="15"/>
+      <c r="CM32" s="15"/>
+      <c r="CN32" s="15"/>
+      <c r="CO32" s="15"/>
+      <c r="CP32" s="15"/>
+      <c r="CQ32" s="15"/>
+      <c r="CR32" s="15"/>
+      <c r="CS32" s="15"/>
+      <c r="CT32" s="15"/>
+      <c r="CU32" s="15"/>
     </row>
     <row r="33" spans="1:214" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C33" s="26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E33" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F33" s="32">
-        <f t="shared" si="3"/>
-        <v>3.4883720930232558</v>
+        <f t="shared" si="1"/>
+        <v>1.1560693641618498</v>
       </c>
       <c r="G33" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DK33" s="15"/>
-      <c r="DL33" s="15"/>
-      <c r="DM33" s="15"/>
-      <c r="DN33" s="15"/>
-      <c r="DO33" s="15"/>
-      <c r="DP33" s="15"/>
+        <f>D33/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="CV33" s="15"/>
+      <c r="CW33" s="15"/>
     </row>
     <row r="34" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>50</v>
+      <c r="B34" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C34" s="26">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E34" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="32">
-        <f t="shared" si="3"/>
-        <v>11.627906976744185</v>
+        <f t="shared" si="1"/>
+        <v>3.4682080924855492</v>
       </c>
       <c r="G34" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DU34" s="17"/>
-      <c r="DV34" s="17"/>
-      <c r="DW34" s="17"/>
-      <c r="DX34" s="17"/>
-      <c r="DY34" s="17"/>
-      <c r="DZ34" s="17"/>
-      <c r="EA34" s="17"/>
-      <c r="EB34" s="17"/>
-      <c r="EC34" s="17"/>
-      <c r="ED34" s="17"/>
-      <c r="EY34" s="17"/>
-      <c r="EZ34" s="17"/>
-      <c r="FA34" s="17"/>
-      <c r="FB34" s="17"/>
-      <c r="FC34" s="17"/>
-      <c r="FD34" s="17"/>
-      <c r="FE34" s="17"/>
-      <c r="FF34" s="17"/>
-      <c r="FG34" s="17"/>
-      <c r="FH34" s="17"/>
+        <f>D34/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="DK34" s="15"/>
+      <c r="DL34" s="15"/>
+      <c r="DM34" s="15"/>
+      <c r="DN34" s="15"/>
+      <c r="DO34" s="15"/>
+      <c r="DP34" s="15"/>
     </row>
     <row r="35" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="B35" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="26">
+        <v>20</v>
+      </c>
+      <c r="E35" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="32">
+        <f t="shared" si="1"/>
+        <v>11.560693641618498</v>
+      </c>
+      <c r="G35" s="32">
+        <f>D35/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="DU35" s="17"/>
+      <c r="DV35" s="17"/>
+      <c r="DW35" s="17"/>
+      <c r="DX35" s="17"/>
+      <c r="DY35" s="17"/>
+      <c r="DZ35" s="17"/>
+      <c r="EA35" s="17"/>
+      <c r="EB35" s="17"/>
+      <c r="EC35" s="17"/>
+      <c r="ED35" s="17"/>
+      <c r="EY35" s="17"/>
+      <c r="EZ35" s="17"/>
+      <c r="FA35" s="17"/>
+      <c r="FB35" s="17"/>
+      <c r="FC35" s="17"/>
+      <c r="FD35" s="17"/>
+      <c r="FE35" s="17"/>
+      <c r="FF35" s="17"/>
+      <c r="FG35" s="17"/>
+      <c r="FH35" s="17"/>
+    </row>
+    <row r="36" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="25">
-        <f>SUM(C36:C36)</f>
+      <c r="B36" s="19"/>
+      <c r="C36" s="25">
+        <f>SUM(C37:C37)</f>
         <v>15</v>
       </c>
-      <c r="D35" s="25">
-        <f>SUM(D36:D36)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="41">
+      <c r="D36" s="25">
+        <f>SUM(D37:D37)</f>
+        <v>6</v>
+      </c>
+      <c r="E36" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="31">
-        <f t="shared" si="3"/>
-        <v>8.720930232558139</v>
-      </c>
-      <c r="G35" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="20" t="str">
-        <f>IF(MIN(H36)=0,"-",MIN(H36))</f>
+        <v>9</v>
+      </c>
+      <c r="F36" s="31">
+        <f t="shared" si="1"/>
+        <v>8.6705202312138727</v>
+      </c>
+      <c r="G36" s="31">
+        <f>D36/($D$53/100)</f>
+        <v>24.489795918367346</v>
+      </c>
+      <c r="H36" s="20">
+        <f>IF(MIN(H37)=0,"-",MIN(H37))</f>
+        <v>45220</v>
+      </c>
+      <c r="I36" s="20" t="str">
+        <f>IF(MAX(I37)=0,"-",MAX(I37))</f>
         <v>-</v>
       </c>
-      <c r="I35" s="20" t="str">
-        <f>IF(MAX(I36)=0,"-",MAX(I36))</f>
+      <c r="AY36" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ36" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB36" s="13"/>
+      <c r="BC36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE36" s="13"/>
+      <c r="BF36" s="13"/>
+      <c r="BG36" s="13"/>
+      <c r="BH36" s="13"/>
+      <c r="BI36" s="13"/>
+      <c r="BJ36" s="13"/>
+      <c r="BK36" s="13"/>
+      <c r="BL36" s="13"/>
+      <c r="BM36" s="13"/>
+      <c r="BN36" s="13"/>
+      <c r="BO36" s="13"/>
+      <c r="BP36" s="13"/>
+      <c r="BQ36" s="13"/>
+      <c r="BR36" s="13"/>
+      <c r="BS36" s="13"/>
+      <c r="BT36" s="13"/>
+      <c r="BU36" s="13"/>
+      <c r="BV36" s="13"/>
+      <c r="BW36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BX36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="BY36" s="13"/>
+      <c r="BZ36" s="13"/>
+      <c r="CA36" s="13"/>
+      <c r="CB36" s="13"/>
+      <c r="CC36" s="13"/>
+      <c r="CD36" s="13"/>
+      <c r="CE36" s="13"/>
+      <c r="CF36" s="13"/>
+      <c r="CG36" s="13"/>
+      <c r="CH36" s="13"/>
+      <c r="CI36" s="13"/>
+      <c r="CJ36" s="13"/>
+      <c r="CK36" s="13"/>
+      <c r="CL36" s="13"/>
+      <c r="CM36" s="13"/>
+      <c r="CN36" s="13"/>
+      <c r="CO36" s="13"/>
+      <c r="CP36" s="13"/>
+      <c r="CQ36" s="13"/>
+      <c r="CR36" s="13"/>
+      <c r="CS36" s="13"/>
+      <c r="CT36" s="13"/>
+      <c r="CU36" s="13"/>
+      <c r="CV36" s="13"/>
+      <c r="CW36" s="13"/>
+      <c r="CX36" s="13"/>
+      <c r="CY36" s="13"/>
+      <c r="CZ36" s="13"/>
+      <c r="DA36" s="13"/>
+      <c r="DB36" s="13"/>
+      <c r="DC36" s="13"/>
+      <c r="DD36" s="13"/>
+      <c r="DE36" s="13"/>
+      <c r="DF36" s="13"/>
+      <c r="DG36" s="13"/>
+      <c r="DH36" s="13"/>
+      <c r="DI36" s="13"/>
+      <c r="DJ36" s="13"/>
+      <c r="DK36" s="13"/>
+      <c r="DL36" s="13"/>
+      <c r="DM36" s="13"/>
+      <c r="DN36" s="13"/>
+      <c r="DO36" s="13"/>
+      <c r="DP36" s="13"/>
+      <c r="DQ36" s="13"/>
+      <c r="DR36" s="13"/>
+      <c r="DS36" s="13"/>
+      <c r="DT36" s="13"/>
+      <c r="DU36" s="13"/>
+      <c r="DV36" s="13"/>
+      <c r="DW36" s="13"/>
+      <c r="DX36" s="13"/>
+      <c r="DY36" s="13"/>
+    </row>
+    <row r="37" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="26">
+        <v>15</v>
+      </c>
+      <c r="D37" s="26">
+        <v>6</v>
+      </c>
+      <c r="E37" s="42">
+        <v>4</v>
+      </c>
+      <c r="F37" s="32">
+        <f t="shared" si="1"/>
+        <v>8.6705202312138727</v>
+      </c>
+      <c r="G37" s="32">
+        <f>D37/($D$53/100)</f>
+        <v>24.489795918367346</v>
+      </c>
+      <c r="H37" s="18">
+        <v>45220</v>
+      </c>
+      <c r="AY37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB37" s="15"/>
+      <c r="BC37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL37" s="15"/>
+      <c r="BV37" s="15"/>
+      <c r="BW37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BX37" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="CF37" s="15"/>
+      <c r="CP37" s="15"/>
+      <c r="CZ37" s="15"/>
+      <c r="DF37" s="15"/>
+      <c r="DG37" s="15"/>
+      <c r="DQ37" s="15"/>
+      <c r="DR37" s="15"/>
+      <c r="DU37" s="15"/>
+      <c r="DV37" s="15"/>
+      <c r="DW37" s="15"/>
+      <c r="DX37" s="15"/>
+      <c r="DY37" s="15"/>
+    </row>
+    <row r="38" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="33">
+        <f>D38/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="10">
+        <v>45276</v>
+      </c>
+      <c r="I38" s="10"/>
+      <c r="DZ38" s="16"/>
+    </row>
+    <row r="39" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="25">
+        <f>SUM(C40:C42)</f>
+        <v>7</v>
+      </c>
+      <c r="D39" s="25">
+        <f>SUM(D40:D42)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="31">
+        <f t="shared" si="1"/>
+        <v>4.0462427745664744</v>
+      </c>
+      <c r="G39" s="31">
+        <f>D39/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="20" t="str">
+        <f>IF(MIN(H40:H42)=0,"-",MIN(H40:H42))</f>
         <v>-</v>
       </c>
-      <c r="BB35" s="13"/>
-      <c r="BC35" s="13"/>
-      <c r="BD35" s="13"/>
-      <c r="BE35" s="13"/>
-      <c r="BF35" s="13"/>
-      <c r="BG35" s="13"/>
-      <c r="BH35" s="13"/>
-      <c r="BI35" s="13"/>
-      <c r="BJ35" s="13"/>
-      <c r="BK35" s="13"/>
-      <c r="BL35" s="13"/>
-      <c r="BM35" s="13"/>
-      <c r="BN35" s="13"/>
-      <c r="BO35" s="13"/>
-      <c r="BP35" s="13"/>
-      <c r="BQ35" s="13"/>
-      <c r="BR35" s="13"/>
-      <c r="BS35" s="13"/>
-      <c r="BT35" s="13"/>
-      <c r="BU35" s="13"/>
-      <c r="BV35" s="13"/>
-      <c r="BW35" s="13"/>
-      <c r="BX35" s="13"/>
-      <c r="BY35" s="13"/>
-      <c r="BZ35" s="13"/>
-      <c r="CA35" s="13"/>
-      <c r="CB35" s="13"/>
-      <c r="CC35" s="13"/>
-      <c r="CD35" s="13"/>
-      <c r="CE35" s="13"/>
-      <c r="CF35" s="13"/>
-      <c r="CG35" s="13"/>
-      <c r="CH35" s="13"/>
-      <c r="CI35" s="13"/>
-      <c r="CJ35" s="13"/>
-      <c r="CK35" s="13"/>
-      <c r="CL35" s="13"/>
-      <c r="CM35" s="13"/>
-      <c r="CN35" s="13"/>
-      <c r="CO35" s="13"/>
-      <c r="CP35" s="13"/>
-      <c r="CQ35" s="13"/>
-      <c r="CR35" s="13"/>
-      <c r="CS35" s="13"/>
-      <c r="CT35" s="13"/>
-      <c r="CU35" s="13"/>
-      <c r="CV35" s="13"/>
-      <c r="CW35" s="13"/>
-      <c r="CX35" s="13"/>
-      <c r="CY35" s="13"/>
-      <c r="CZ35" s="13"/>
-      <c r="DA35" s="13"/>
-      <c r="DB35" s="13"/>
-      <c r="DC35" s="13"/>
-      <c r="DD35" s="13"/>
-      <c r="DE35" s="13"/>
-      <c r="DF35" s="13"/>
-      <c r="DG35" s="13"/>
-      <c r="DH35" s="13"/>
-      <c r="DI35" s="13"/>
-      <c r="DJ35" s="13"/>
-      <c r="DK35" s="13"/>
-      <c r="DL35" s="13"/>
-      <c r="DM35" s="13"/>
-      <c r="DN35" s="13"/>
-      <c r="DO35" s="13"/>
-      <c r="DP35" s="13"/>
-      <c r="DQ35" s="13"/>
-      <c r="DR35" s="13"/>
-      <c r="DS35" s="13"/>
-      <c r="DT35" s="13"/>
-      <c r="DU35" s="13"/>
-      <c r="DV35" s="13"/>
-      <c r="DW35" s="13"/>
-      <c r="DX35" s="13"/>
-      <c r="DY35" s="13"/>
-    </row>
-    <row r="36" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="26">
-        <v>15</v>
-      </c>
-      <c r="E36" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="32">
-        <f t="shared" si="3"/>
-        <v>8.720930232558139</v>
-      </c>
-      <c r="G36" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="BB36" s="15"/>
-      <c r="BL36" s="15"/>
-      <c r="BV36" s="15"/>
-      <c r="CF36" s="15"/>
-      <c r="CP36" s="15"/>
-      <c r="CZ36" s="15"/>
-      <c r="DF36" s="15"/>
-      <c r="DG36" s="15"/>
-      <c r="DQ36" s="15"/>
-      <c r="DR36" s="15"/>
-      <c r="DU36" s="15"/>
-      <c r="DV36" s="15"/>
-      <c r="DW36" s="15"/>
-      <c r="DX36" s="15"/>
-      <c r="DY36" s="15"/>
-    </row>
-    <row r="37" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="10">
-        <v>45276</v>
-      </c>
-      <c r="I37" s="10"/>
-      <c r="DZ37" s="16"/>
-    </row>
-    <row r="38" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="25">
-        <f>SUM(C39:C41)</f>
-        <v>7</v>
-      </c>
-      <c r="D38" s="25">
-        <f>SUM(D39:D41)</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="31">
-        <f t="shared" si="3"/>
-        <v>4.0697674418604652</v>
-      </c>
-      <c r="G38" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="20" t="str">
-        <f>IF(MIN(H39:H41)=0,"-",MIN(H39:H41))</f>
+      <c r="I39" s="20" t="str">
+        <f>IF(MAX(I40:I42)=0,"-",MAX(I40:I42))</f>
         <v>-</v>
       </c>
-      <c r="I38" s="20" t="str">
-        <f>IF(MAX(I39:I41)=0,"-",MAX(I39:I41))</f>
-        <v>-</v>
-      </c>
-      <c r="AS38" s="53"/>
-      <c r="AT38" s="53"/>
-      <c r="AU38" s="53"/>
-      <c r="AV38" s="53"/>
-      <c r="AW38" s="53"/>
-      <c r="AX38" s="53"/>
-      <c r="AY38" s="13"/>
-      <c r="AZ38" s="13"/>
-      <c r="BA38" s="13"/>
-      <c r="BB38" s="13"/>
-      <c r="BC38" s="13"/>
-      <c r="BD38" s="13"/>
-      <c r="BE38" s="13"/>
-      <c r="BF38" s="13"/>
-      <c r="BG38" s="13"/>
-      <c r="BH38" s="13"/>
-      <c r="BI38" s="13"/>
-      <c r="BJ38" s="13"/>
-      <c r="BK38" s="13"/>
-      <c r="BL38" s="13"/>
-      <c r="BM38" s="13"/>
-      <c r="BN38" s="13"/>
-      <c r="BO38" s="13"/>
-      <c r="BP38" s="13"/>
-      <c r="BQ38" s="13"/>
-      <c r="BR38" s="13"/>
-      <c r="BS38" s="13"/>
-      <c r="BT38" s="13"/>
-      <c r="BU38" s="13"/>
-      <c r="BV38" s="13"/>
-      <c r="BW38" s="13"/>
-      <c r="BX38" s="13"/>
-      <c r="BY38" s="13"/>
-      <c r="BZ38" s="13"/>
-      <c r="CA38" s="13"/>
-      <c r="CB38" s="13"/>
-      <c r="CC38" s="13"/>
-      <c r="CD38" s="13"/>
-      <c r="CE38" s="13"/>
-      <c r="CF38" s="13"/>
-      <c r="CG38" s="13"/>
-      <c r="CH38" s="13"/>
-      <c r="CI38" s="13"/>
-      <c r="CJ38" s="13"/>
-      <c r="CK38" s="13"/>
-      <c r="CL38" s="13"/>
-      <c r="CM38" s="13"/>
-      <c r="CN38" s="13"/>
-      <c r="CO38" s="13"/>
-      <c r="CP38" s="13"/>
-      <c r="CQ38" s="13"/>
-      <c r="CR38" s="13"/>
-      <c r="CS38" s="13"/>
-      <c r="CT38" s="13"/>
-      <c r="CU38" s="13"/>
-      <c r="CV38" s="13"/>
-      <c r="CW38" s="13"/>
-      <c r="CX38" s="13"/>
-      <c r="CY38" s="13"/>
-      <c r="CZ38" s="13"/>
-      <c r="DA38" s="13"/>
-      <c r="DB38" s="13"/>
-      <c r="DC38" s="13"/>
-      <c r="DD38" s="13"/>
-      <c r="DE38" s="13"/>
-    </row>
-    <row r="39" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="26">
-        <v>2</v>
-      </c>
-      <c r="E39" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="32">
-        <f t="shared" si="3"/>
-        <v>1.1627906976744187</v>
-      </c>
-      <c r="G39" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AY39" s="15"/>
-      <c r="AZ39" s="15"/>
+      <c r="AY39" s="13"/>
+      <c r="AZ39" s="13"/>
+      <c r="BA39" s="13"/>
+      <c r="BB39" s="13"/>
+      <c r="BC39" s="13"/>
+      <c r="BD39" s="13"/>
+      <c r="BE39" s="13"/>
+      <c r="BF39" s="13"/>
+      <c r="BG39" s="13"/>
+      <c r="BH39" s="13"/>
+      <c r="BI39" s="13"/>
+      <c r="BJ39" s="13"/>
+      <c r="BK39" s="13"/>
+      <c r="BL39" s="13"/>
+      <c r="BM39" s="13"/>
+      <c r="BN39" s="13"/>
+      <c r="BO39" s="13"/>
+      <c r="BP39" s="13"/>
+      <c r="BQ39" s="13"/>
+      <c r="BR39" s="13"/>
+      <c r="BS39" s="13"/>
+      <c r="BT39" s="13"/>
+      <c r="BU39" s="13"/>
+      <c r="BV39" s="13"/>
+      <c r="BW39" s="13"/>
+      <c r="BX39" s="13"/>
+      <c r="BY39" s="13"/>
+      <c r="BZ39" s="13"/>
+      <c r="CA39" s="13"/>
+      <c r="CB39" s="13"/>
+      <c r="CC39" s="13"/>
+      <c r="CD39" s="13"/>
+      <c r="CE39" s="13"/>
+      <c r="CF39" s="13"/>
+      <c r="CG39" s="13"/>
+      <c r="CH39" s="13"/>
+      <c r="CI39" s="13"/>
+      <c r="CJ39" s="13"/>
+      <c r="CK39" s="13"/>
+      <c r="CL39" s="13"/>
+      <c r="CM39" s="13"/>
+      <c r="CN39" s="13"/>
+      <c r="CO39" s="13"/>
+      <c r="CP39" s="13"/>
+      <c r="CQ39" s="13"/>
+      <c r="CR39" s="13"/>
+      <c r="CS39" s="13"/>
+      <c r="CT39" s="13"/>
+      <c r="CU39" s="13"/>
+      <c r="CV39" s="13"/>
+      <c r="CW39" s="13"/>
+      <c r="CX39" s="13"/>
+      <c r="CY39" s="13"/>
+      <c r="CZ39" s="13"/>
+      <c r="DA39" s="13"/>
+      <c r="DB39" s="13"/>
+      <c r="DC39" s="13"/>
+      <c r="DD39" s="13"/>
+      <c r="DE39" s="13"/>
     </row>
     <row r="40" spans="1:214" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F40" s="32">
-        <f t="shared" si="3"/>
-        <v>1.7441860465116279</v>
+        <f t="shared" si="1"/>
+        <v>1.1560693641618498</v>
       </c>
       <c r="G40" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AU40" s="53"/>
-      <c r="BA40" s="15"/>
-      <c r="DB40" s="15"/>
-      <c r="DC40" s="15"/>
+        <f>D40/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AY40" s="15"/>
+      <c r="AZ40" s="15"/>
     </row>
     <row r="41" spans="1:214" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F41" s="32">
-        <f t="shared" si="3"/>
-        <v>1.1627906976744187</v>
+        <f t="shared" si="1"/>
+        <v>1.7341040462427746</v>
       </c>
       <c r="G41" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DD41" s="15"/>
-      <c r="DE41" s="15"/>
+        <f>D41/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="BA41" s="15"/>
+      <c r="DB41" s="15"/>
+      <c r="DC41" s="15"/>
     </row>
     <row r="42" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="B42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="26">
+        <v>2</v>
+      </c>
+      <c r="E42" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
+        <f t="shared" si="1"/>
+        <v>1.1560693641618498</v>
+      </c>
+      <c r="G42" s="32">
+        <f>D42/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="DD42" s="15"/>
+      <c r="DE42" s="15"/>
+    </row>
+    <row r="43" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="43">
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F42" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H42" s="10">
+      <c r="F43" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="33">
+        <f>D43/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="10">
         <v>45296</v>
       </c>
-      <c r="I42" s="10"/>
-      <c r="FC42" s="16"/>
-    </row>
-    <row r="43" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="I43" s="10"/>
+      <c r="FC43" s="16"/>
+    </row>
+    <row r="44" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="25">
-        <f>SUM(C44:C45)</f>
+      <c r="B44" s="19"/>
+      <c r="C44" s="25">
+        <f>SUM(C45:C46)</f>
         <v>2</v>
       </c>
-      <c r="D43" s="25">
-        <f>SUM(D44:D45)</f>
-        <v>0</v>
-      </c>
-      <c r="E43" s="41">
+      <c r="D44" s="25">
+        <f>SUM(D45:D46)</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F43" s="31">
-        <f t="shared" si="3"/>
-        <v>1.1627906976744187</v>
-      </c>
-      <c r="G43" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H43" s="20" t="str">
-        <f>IF(MIN(H44:H45)=0,"-",MIN(H44:H45))</f>
+      <c r="F44" s="31">
+        <f t="shared" si="1"/>
+        <v>1.1560693641618498</v>
+      </c>
+      <c r="G44" s="31">
+        <f>D44/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="20" t="str">
+        <f>IF(MIN(H45:H46)=0,"-",MIN(H45:H46))</f>
         <v>-</v>
       </c>
-      <c r="I43" s="20" t="str">
-        <f>IF(MAX(I44:I45)=0,"-",MAX(I44:I45))</f>
+      <c r="I44" s="20" t="str">
+        <f>IF(MAX(I45:I46)=0,"-",MAX(I45:I46))</f>
         <v>-</v>
       </c>
-      <c r="EY43" s="13"/>
-      <c r="EZ43" s="13"/>
-    </row>
-    <row r="44" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="E44" s="42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="32">
-        <f t="shared" si="3"/>
-        <v>0.29069767441860467</v>
-      </c>
-      <c r="G44" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="EY44" s="15"/>
+      <c r="EY44" s="13"/>
+      <c r="EZ44" s="13"/>
     </row>
     <row r="45" spans="1:214" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C45" s="26">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F45" s="32">
-        <f t="shared" si="3"/>
-        <v>0.87209302325581395</v>
+        <f t="shared" si="1"/>
+        <v>0.28901734104046245</v>
       </c>
       <c r="G45" s="32">
-        <f t="shared" si="2"/>
+        <f>D45/($D$53/100)</f>
         <v>0</v>
       </c>
       <c r="EY45" s="15"/>
-      <c r="EZ45" s="15"/>
     </row>
     <row r="46" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="B46" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="26">
+        <v>1.5</v>
+      </c>
+      <c r="E46" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="32">
+        <f t="shared" si="1"/>
+        <v>0.86705202312138729</v>
+      </c>
+      <c r="G46" s="32">
+        <f>D46/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="EY46" s="15"/>
+      <c r="EZ46" s="15"/>
+    </row>
+    <row r="47" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H46" s="10">
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="33">
+        <f>D47/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="10">
         <v>45332</v>
       </c>
-      <c r="I46" s="10"/>
-      <c r="HF46" s="16"/>
-    </row>
-    <row r="47" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="I47" s="10"/>
+      <c r="HF47" s="16"/>
+    </row>
+    <row r="48" spans="1:214" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="19"/>
-      <c r="C47" s="25">
-        <f>SUM(C48:C48)</f>
+      <c r="B48" s="19"/>
+      <c r="C48" s="25">
+        <f>SUM(C49:C49)</f>
         <v>3</v>
       </c>
-      <c r="D47" s="25">
-        <f t="shared" ref="D47" si="4">SUM(D48:D48)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="41">
-        <f>IF(C47-D47=C47,0,C47-D47)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="31">
-        <f t="shared" si="3"/>
-        <v>1.7441860465116279</v>
-      </c>
-      <c r="G47" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H47" s="20" t="str">
-        <f>IF(MIN(H48)=0,"-",MIN(H48))</f>
+      <c r="D48" s="25">
+        <f t="shared" ref="D48" si="2">SUM(D49:D49)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="41">
+        <f>IF(C48-D48=C48,0,C48-D48)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="31">
+        <f t="shared" si="1"/>
+        <v>1.7341040462427746</v>
+      </c>
+      <c r="G48" s="31">
+        <f>D48/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="20" t="str">
+        <f>IF(MIN(H49)=0,"-",MIN(H49))</f>
         <v>-</v>
       </c>
-      <c r="I47" s="20" t="str">
-        <f>IF(MAX(I48)=0,"-",MAX(I48))</f>
+      <c r="I48" s="20" t="str">
+        <f>IF(MAX(I49)=0,"-",MAX(I49))</f>
         <v>-</v>
       </c>
-      <c r="FI47" s="13"/>
-      <c r="FJ47" s="13"/>
-      <c r="FK47" s="13"/>
-    </row>
-    <row r="48" spans="1:214" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
+      <c r="FI48" s="13"/>
+      <c r="FJ48" s="13"/>
+      <c r="FK48" s="13"/>
+    </row>
+    <row r="49" spans="1:227" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="26">
+      <c r="C49" s="26">
         <v>3</v>
       </c>
-      <c r="D48" s="29"/>
-      <c r="E48" s="42">
-        <f>IF(C48-D48=C48,0,C48-D48)</f>
-        <v>0</v>
-      </c>
-      <c r="F48" s="32">
-        <f t="shared" si="3"/>
-        <v>1.7441860465116279</v>
-      </c>
-      <c r="G48" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="FI48" s="15"/>
-      <c r="FJ48" s="15"/>
-      <c r="FK48" s="15"/>
-    </row>
-    <row r="49" spans="1:227" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="D49" s="29"/>
+      <c r="E49" s="42">
+        <f>IF(C49-D49=C49,0,C49-D49)</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="32">
+        <f t="shared" si="1"/>
+        <v>1.7341040462427746</v>
+      </c>
+      <c r="G49" s="32">
+        <f>D49/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="FI49" s="15"/>
+      <c r="FJ49" s="15"/>
+      <c r="FK49" s="15"/>
+    </row>
+    <row r="50" spans="1:227" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="28">
+      <c r="B50" s="11"/>
+      <c r="C50" s="28">
         <v>44</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="44">
+      <c r="D50" s="28"/>
+      <c r="E50" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F49" s="34">
-        <f t="shared" si="3"/>
-        <v>25.581395348837209</v>
-      </c>
-      <c r="G49" s="34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="FN49" s="17"/>
-      <c r="FO49" s="17"/>
-      <c r="FP49" s="17"/>
-      <c r="FQ49" s="17"/>
-      <c r="FR49" s="17"/>
-      <c r="FS49" s="17"/>
-      <c r="FT49" s="17"/>
-      <c r="FU49" s="17"/>
-      <c r="FV49" s="17"/>
-      <c r="FW49" s="17"/>
-      <c r="FX49" s="17"/>
-      <c r="FY49" s="17"/>
-      <c r="FZ49" s="17"/>
-      <c r="GA49" s="17"/>
-      <c r="GB49" s="17"/>
-      <c r="GC49" s="17"/>
-      <c r="GD49" s="17"/>
-      <c r="GE49" s="17"/>
-      <c r="GF49" s="17"/>
-      <c r="GG49" s="17"/>
-      <c r="GH49" s="17"/>
-      <c r="GI49" s="17"/>
-      <c r="GJ49" s="17"/>
-      <c r="GK49" s="17"/>
-      <c r="GL49" s="17"/>
-      <c r="GM49" s="17"/>
-      <c r="GN49" s="17"/>
-      <c r="GO49" s="17"/>
-      <c r="GP49" s="17"/>
-      <c r="GQ49" s="17"/>
-      <c r="GR49" s="17"/>
-      <c r="GS49" s="17"/>
-      <c r="GT49" s="17"/>
-      <c r="GU49" s="17"/>
-      <c r="GV49" s="17"/>
-      <c r="GW49" s="17"/>
-      <c r="GX49" s="17"/>
-      <c r="GY49" s="17"/>
-      <c r="GZ49" s="17"/>
-      <c r="HA49" s="17"/>
-      <c r="HB49" s="17"/>
-      <c r="HC49" s="17"/>
-      <c r="HD49" s="17"/>
-      <c r="HE49" s="17"/>
-    </row>
-    <row r="50" spans="1:227" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="F50" s="34">
+        <f t="shared" si="1"/>
+        <v>25.433526011560694</v>
+      </c>
+      <c r="G50" s="34">
+        <f>D50/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="FN50" s="17"/>
+      <c r="FO50" s="17"/>
+      <c r="FP50" s="17"/>
+      <c r="FQ50" s="17"/>
+      <c r="FR50" s="17"/>
+      <c r="FS50" s="17"/>
+      <c r="FT50" s="17"/>
+      <c r="FU50" s="17"/>
+      <c r="FV50" s="17"/>
+      <c r="FW50" s="17"/>
+      <c r="FX50" s="17"/>
+      <c r="FY50" s="17"/>
+      <c r="FZ50" s="17"/>
+      <c r="GA50" s="17"/>
+      <c r="GB50" s="17"/>
+      <c r="GC50" s="17"/>
+      <c r="GD50" s="17"/>
+      <c r="GE50" s="17"/>
+      <c r="GF50" s="17"/>
+      <c r="GG50" s="17"/>
+      <c r="GH50" s="17"/>
+      <c r="GI50" s="17"/>
+      <c r="GJ50" s="17"/>
+      <c r="GK50" s="17"/>
+      <c r="GL50" s="17"/>
+      <c r="GM50" s="17"/>
+      <c r="GN50" s="17"/>
+      <c r="GO50" s="17"/>
+      <c r="GP50" s="17"/>
+      <c r="GQ50" s="17"/>
+      <c r="GR50" s="17"/>
+      <c r="GS50" s="17"/>
+      <c r="GT50" s="17"/>
+      <c r="GU50" s="17"/>
+      <c r="GV50" s="17"/>
+      <c r="GW50" s="17"/>
+      <c r="GX50" s="17"/>
+      <c r="GY50" s="17"/>
+      <c r="GZ50" s="17"/>
+      <c r="HA50" s="17"/>
+      <c r="HB50" s="17"/>
+      <c r="HC50" s="17"/>
+      <c r="HD50" s="17"/>
+      <c r="HE50" s="17"/>
+    </row>
+    <row r="51" spans="1:227" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="33">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H50" s="10">
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="33">
+        <f>D51/($D$53/100)</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="10">
         <v>45345</v>
       </c>
-      <c r="I50" s="10"/>
-      <c r="HS50" s="16"/>
-    </row>
-    <row r="51" spans="1:227" x14ac:dyDescent="0.25">
-      <c r="F51" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:227" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="I51" s="10"/>
+      <c r="HS51" s="16"/>
+    </row>
+    <row r="52" spans="1:227" x14ac:dyDescent="0.25">
+      <c r="F52" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="32">
+        <f>D52/($D$53/100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:227" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37">
-        <f>SUM(C2:C51)-SUM(C2,C7,C15,C21,C35,C38,C43,C47)</f>
-        <v>172</v>
-      </c>
-      <c r="D52" s="37">
-        <f>SUM(D2:D51)-SUM(D2,D7,D15,D21,D35,D38,D43,D47)</f>
-        <v>13</v>
-      </c>
-      <c r="E52" s="45">
-        <f>C52-D52-SUM(E2:E51)+SUM(E2,E7,E15,E21,E35,E38,E43,E47)</f>
-        <v>151</v>
-      </c>
-      <c r="F52" s="38">
-        <f t="shared" si="3"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="37">
+        <f>SUM(C2:C52)-SUM(C2,C7,C15,C22,C36,C39,C44,C48)</f>
+        <v>173</v>
+      </c>
+      <c r="D53" s="37">
+        <f>SUM(D2:D52)-SUM(D2,D7,D15,D22,D36,D39,D44,D48)</f>
+        <v>24.5</v>
+      </c>
+      <c r="E53" s="45" t="e">
+        <f>C53-D53-SUM(E2:E52)+SUM(E2,E7,E15,E22,E36,E39,E44,E48)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F53" s="38">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G52" s="38">
-        <f t="shared" si="2"/>
+      <c r="G53" s="38">
+        <f>D53/($D$53/100)</f>
         <v>100</v>
       </c>
-      <c r="H52" s="39">
-        <f>IF(MIN(H1:H51)=0,"-",MIN(H1:H51))</f>
+      <c r="H53" s="39">
+        <f>IF(MIN(H1:H52)=0,"-",MIN(H1:H52))</f>
         <v>45198</v>
       </c>
-      <c r="I52" s="39">
-        <f>MAX(I2:I51)</f>
-        <v>45219</v>
+      <c r="I53" s="39">
+        <f>MAX(I2:I52)</f>
+        <v>45240</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="NF1:NJ1"/>
-    <mergeCell ref="NK1:NO1"/>
-    <mergeCell ref="NP1:NT1"/>
-    <mergeCell ref="MB1:MF1"/>
-    <mergeCell ref="MG1:MK1"/>
-    <mergeCell ref="ML1:MP1"/>
-    <mergeCell ref="MQ1:MU1"/>
-    <mergeCell ref="MV1:MZ1"/>
-    <mergeCell ref="NA1:NE1"/>
+    <mergeCell ref="AI1:AM1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="CQ1:CU1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="AS1:AW1"/>
+    <mergeCell ref="AX1:BB1"/>
+    <mergeCell ref="BC1:BG1"/>
+    <mergeCell ref="BH1:BL1"/>
+    <mergeCell ref="BM1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:CA1"/>
+    <mergeCell ref="CB1:CF1"/>
+    <mergeCell ref="CG1:CK1"/>
+    <mergeCell ref="CL1:CP1"/>
+    <mergeCell ref="EY1:FC1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DA1:DE1"/>
+    <mergeCell ref="DF1:DJ1"/>
+    <mergeCell ref="DK1:DO1"/>
+    <mergeCell ref="DP1:DT1"/>
+    <mergeCell ref="DU1:DY1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="EE1:EI1"/>
+    <mergeCell ref="EJ1:EN1"/>
+    <mergeCell ref="EO1:ES1"/>
+    <mergeCell ref="ET1:EX1"/>
+    <mergeCell ref="HG1:HK1"/>
+    <mergeCell ref="FD1:FH1"/>
+    <mergeCell ref="FI1:FM1"/>
+    <mergeCell ref="FN1:FR1"/>
+    <mergeCell ref="FS1:FW1"/>
+    <mergeCell ref="FX1:GB1"/>
+    <mergeCell ref="GC1:GG1"/>
+    <mergeCell ref="GH1:GL1"/>
+    <mergeCell ref="GM1:GQ1"/>
+    <mergeCell ref="GR1:GV1"/>
+    <mergeCell ref="GW1:HA1"/>
+    <mergeCell ref="HB1:HF1"/>
+    <mergeCell ref="JO1:JS1"/>
+    <mergeCell ref="HL1:HP1"/>
+    <mergeCell ref="HQ1:HU1"/>
+    <mergeCell ref="HV1:HZ1"/>
+    <mergeCell ref="IA1:IE1"/>
+    <mergeCell ref="IF1:IJ1"/>
+    <mergeCell ref="IK1:IO1"/>
+    <mergeCell ref="IP1:IT1"/>
+    <mergeCell ref="IU1:IY1"/>
+    <mergeCell ref="IZ1:JD1"/>
+    <mergeCell ref="JE1:JI1"/>
+    <mergeCell ref="JJ1:JN1"/>
     <mergeCell ref="LW1:MA1"/>
     <mergeCell ref="JT1:JX1"/>
     <mergeCell ref="JY1:KC1"/>
@@ -4634,60 +4823,15 @@
     <mergeCell ref="LH1:LL1"/>
     <mergeCell ref="LM1:LQ1"/>
     <mergeCell ref="LR1:LV1"/>
-    <mergeCell ref="JO1:JS1"/>
-    <mergeCell ref="HL1:HP1"/>
-    <mergeCell ref="HQ1:HU1"/>
-    <mergeCell ref="HV1:HZ1"/>
-    <mergeCell ref="IA1:IE1"/>
-    <mergeCell ref="IF1:IJ1"/>
-    <mergeCell ref="IK1:IO1"/>
-    <mergeCell ref="IP1:IT1"/>
-    <mergeCell ref="IU1:IY1"/>
-    <mergeCell ref="IZ1:JD1"/>
-    <mergeCell ref="JE1:JI1"/>
-    <mergeCell ref="JJ1:JN1"/>
-    <mergeCell ref="HG1:HK1"/>
-    <mergeCell ref="FD1:FH1"/>
-    <mergeCell ref="FI1:FM1"/>
-    <mergeCell ref="FN1:FR1"/>
-    <mergeCell ref="FS1:FW1"/>
-    <mergeCell ref="FX1:GB1"/>
-    <mergeCell ref="GC1:GG1"/>
-    <mergeCell ref="GH1:GL1"/>
-    <mergeCell ref="GM1:GQ1"/>
-    <mergeCell ref="GR1:GV1"/>
-    <mergeCell ref="GW1:HA1"/>
-    <mergeCell ref="HB1:HF1"/>
-    <mergeCell ref="EY1:FC1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DA1:DE1"/>
-    <mergeCell ref="DF1:DJ1"/>
-    <mergeCell ref="DK1:DO1"/>
-    <mergeCell ref="DP1:DT1"/>
-    <mergeCell ref="DU1:DY1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="EE1:EI1"/>
-    <mergeCell ref="EJ1:EN1"/>
-    <mergeCell ref="EO1:ES1"/>
-    <mergeCell ref="ET1:EX1"/>
-    <mergeCell ref="CQ1:CU1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="AS1:AW1"/>
-    <mergeCell ref="AX1:BB1"/>
-    <mergeCell ref="BC1:BG1"/>
-    <mergeCell ref="BH1:BL1"/>
-    <mergeCell ref="BM1:BQ1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BW1:CA1"/>
-    <mergeCell ref="CB1:CF1"/>
-    <mergeCell ref="CG1:CK1"/>
-    <mergeCell ref="CL1:CP1"/>
-    <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="NF1:NJ1"/>
+    <mergeCell ref="NK1:NO1"/>
+    <mergeCell ref="NP1:NT1"/>
+    <mergeCell ref="MB1:MF1"/>
+    <mergeCell ref="MG1:MK1"/>
+    <mergeCell ref="ML1:MP1"/>
+    <mergeCell ref="MQ1:MU1"/>
+    <mergeCell ref="MV1:MZ1"/>
+    <mergeCell ref="NA1:NE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4713,8 +4857,8 @@
         <v>70</v>
       </c>
       <c r="B1" s="8">
-        <f>SUM('Gantt Aktuell'!C2:C51)-SUM('Gantt Aktuell'!C2,'Gantt Aktuell'!C7,'Gantt Aktuell'!C15,'Gantt Aktuell'!C21,'Gantt Aktuell'!C35,'Gantt Aktuell'!C38,'Gantt Aktuell'!C43,'Gantt Aktuell'!C47)</f>
-        <v>172</v>
+        <f>SUM('Gantt Aktuell'!C2:C52)-SUM('Gantt Aktuell'!C2,'Gantt Aktuell'!C7,'Gantt Aktuell'!C15,'Gantt Aktuell'!C22,'Gantt Aktuell'!C36,'Gantt Aktuell'!C39,'Gantt Aktuell'!C44,'Gantt Aktuell'!C48)</f>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -4722,8 +4866,8 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <f>SUM('Gantt Aktuell'!D2:D51)-SUM('Gantt Aktuell'!D2,'Gantt Aktuell'!D7,'Gantt Aktuell'!D15,'Gantt Aktuell'!D21,'Gantt Aktuell'!D35,'Gantt Aktuell'!D38,'Gantt Aktuell'!D43,'Gantt Aktuell'!D47)</f>
-        <v>13</v>
+        <f>SUM('Gantt Aktuell'!D2:D52)-SUM('Gantt Aktuell'!D2,'Gantt Aktuell'!D7,'Gantt Aktuell'!D15,'Gantt Aktuell'!D22,'Gantt Aktuell'!D36,'Gantt Aktuell'!D39,'Gantt Aktuell'!D44,'Gantt Aktuell'!D48)</f>
+        <v>24.5</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -4755,16 +4899,16 @@
       </c>
       <c r="B3">
         <f>B1-B2</f>
-        <v>159</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="B4">
-        <f>B1-B2-SUM('Gantt Aktuell'!E2:E51)+SUM('Gantt Aktuell'!E2,'Gantt Aktuell'!E7,'Gantt Aktuell'!E15,'Gantt Aktuell'!E21,'Gantt Aktuell'!E35,'Gantt Aktuell'!E38,'Gantt Aktuell'!E43,'Gantt Aktuell'!E47)</f>
-        <v>151</v>
+      <c r="B4" t="e">
+        <f>B1-B2-SUM('Gantt Aktuell'!E2:E52)+SUM('Gantt Aktuell'!E2,'Gantt Aktuell'!E7,'Gantt Aktuell'!E15,'Gantt Aktuell'!E22,'Gantt Aktuell'!E36,'Gantt Aktuell'!E39,'Gantt Aktuell'!E44,'Gantt Aktuell'!E48)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -4772,7 +4916,7 @@
         <v>74</v>
       </c>
       <c r="B6" s="7">
-        <f>IF(MIN('Gantt Aktuell'!H1:H51)=0,"-",MIN('Gantt Aktuell'!H1:H51))</f>
+        <f>IF(MIN('Gantt Aktuell'!H1:H52)=0,"-",MIN('Gantt Aktuell'!H1:H52))</f>
         <v>45198</v>
       </c>
     </row>
@@ -4781,8 +4925,8 @@
         <v>75</v>
       </c>
       <c r="B7" s="7">
-        <f>MAX('Gantt Aktuell'!I2:I51)</f>
-        <v>45219</v>
+        <f>MAX('Gantt Aktuell'!I2:I52)</f>
+        <v>45240</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -4790,7 +4934,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="7">
-        <f>'Gantt Aktuell'!$H50</f>
+        <f>'Gantt Aktuell'!$H51</f>
         <v>45345</v>
       </c>
     </row>
@@ -4798,9 +4942,9 @@
       <c r="A10" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="46" t="e">
         <f>B2/(B4/100)/100</f>
-        <v>8.6092715231788089E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>